<commit_message>
add deck colours, change dimension of font, fix typo
</commit_message>
<xml_diff>
--- a/data/WNRS.xlsx
+++ b/data/WNRS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KayJan\test-app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCDE4E7-9794-4374-8065-2EBAE24A4D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AFA170-018D-4B86-B28F-96E82F8FBB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="829" firstSheet="3" activeTab="9" xr2:uid="{35520F66-FEA5-4575-927A-C3FC8E8C1344}"/>
+    <workbookView xWindow="6720" yWindow="-13710" windowWidth="14745" windowHeight="11685" tabRatio="829" firstSheet="9" activeTab="12" xr2:uid="{35520F66-FEA5-4575-927A-C3FC8E8C1344}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Deck" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="784">
   <si>
     <t>Card</t>
   </si>
@@ -2443,15 +2443,54 @@
   <si>
     <t>Time to fall in love with myself ❤️</t>
   </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Bl</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Br2</t>
+  </si>
+  <si>
+    <t>Br1</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4508,8 +4547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E751FA87-3BEA-40CD-8458-CB61106840D4}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5152,9 +5191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C1E74C7-997C-4C85-8502-804A6B1DB83E}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -5198,7 +5235,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C6" t="s">
         <v>579</v>
@@ -5209,7 +5246,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C7" t="s">
         <v>580</v>
@@ -5220,7 +5257,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>775</v>
       </c>
       <c r="C8" t="s">
         <v>581</v>
@@ -5231,7 +5268,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C9" t="s">
         <v>582</v>
@@ -5242,7 +5279,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C10" t="s">
         <v>583</v>
@@ -5253,7 +5290,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C11" t="s">
         <v>584</v>
@@ -5264,7 +5301,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C12" t="s">
         <v>585</v>
@@ -5275,7 +5312,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C13" t="s">
         <v>586</v>
@@ -5286,7 +5323,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C14" t="s">
         <v>587</v>
@@ -5297,7 +5334,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C15" t="s">
         <v>588</v>
@@ -5308,7 +5345,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C16" t="s">
         <v>589</v>
@@ -5319,7 +5356,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C17" t="s">
         <v>590</v>
@@ -5330,7 +5367,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C18" t="s">
         <v>591</v>
@@ -5341,7 +5378,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C19" t="s">
         <v>592</v>
@@ -5352,7 +5389,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C20" t="s">
         <v>593</v>
@@ -5363,7 +5400,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C21" t="s">
         <v>594</v>
@@ -5374,7 +5411,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C22" t="s">
         <v>595</v>
@@ -5385,7 +5422,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C23" t="s">
         <v>596</v>
@@ -5396,7 +5433,7 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C24" t="s">
         <v>597</v>
@@ -5407,7 +5444,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C25" t="s">
         <v>598</v>
@@ -5418,7 +5455,7 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>775</v>
       </c>
       <c r="C26" t="s">
         <v>599</v>
@@ -5429,7 +5466,7 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C27" t="s">
         <v>600</v>
@@ -5440,7 +5477,7 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C28" t="s">
         <v>601</v>
@@ -5451,7 +5488,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C29" t="s">
         <v>602</v>
@@ -5462,13 +5499,14 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>775</v>
       </c>
       <c r="C30" t="s">
         <v>603</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5734,9 +5772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941E7727-1D5F-48BE-8AE3-2119045C4067}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -5774,7 +5810,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B6" t="s">
         <v>137</v>
@@ -5782,7 +5818,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B7" t="s">
         <v>138</v>
@@ -5790,7 +5826,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B8" t="s">
         <v>139</v>
@@ -5798,7 +5834,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B9" t="s">
         <v>140</v>
@@ -5806,7 +5842,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B10" t="s">
         <v>141</v>
@@ -5814,7 +5850,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B11" t="s">
         <v>142</v>
@@ -5822,7 +5858,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B12" t="s">
         <v>143</v>
@@ -5830,7 +5866,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B13" t="s">
         <v>144</v>
@@ -5838,7 +5874,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B14" t="s">
         <v>145</v>
@@ -5846,7 +5882,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B15" t="s">
         <v>146</v>
@@ -5854,7 +5890,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B16" t="s">
         <v>147</v>
@@ -5862,7 +5898,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B17" t="s">
         <v>148</v>
@@ -5870,7 +5906,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B18" t="s">
         <v>149</v>
@@ -5878,7 +5914,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B19" t="s">
         <v>150</v>
@@ -5886,7 +5922,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B20" t="s">
         <v>151</v>
@@ -5894,7 +5930,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B21" t="s">
         <v>152</v>
@@ -5902,7 +5938,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B22" t="s">
         <v>153</v>
@@ -5910,7 +5946,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B23" t="s">
         <v>154</v>
@@ -5918,7 +5954,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B24" t="s">
         <v>155</v>
@@ -5926,7 +5962,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B25" t="s">
         <v>156</v>
@@ -5934,7 +5970,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B26" t="s">
         <v>157</v>
@@ -5942,7 +5978,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B27" t="s">
         <v>158</v>
@@ -5950,7 +5986,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="B28" t="s">
         <v>159</v>
@@ -5958,7 +5994,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>3</v>
+        <v>783</v>
       </c>
       <c r="B29" t="s">
         <v>160</v>
@@ -5966,7 +6002,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>3</v>
+        <v>783</v>
       </c>
       <c r="B30" t="s">
         <v>161</v>
@@ -5981,7 +6017,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26BB1692-6F6B-4FFF-B841-EEF12529B92E}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -6025,7 +6063,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C6" t="s">
         <v>120</v>
@@ -6036,7 +6074,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C7" t="s">
         <v>121</v>
@@ -6047,7 +6085,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C8" t="s">
         <v>91</v>
@@ -6058,7 +6096,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C9" t="s">
         <v>122</v>
@@ -6069,7 +6107,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C10" t="s">
         <v>123</v>
@@ -6080,7 +6118,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C11" t="s">
         <v>124</v>
@@ -6091,7 +6129,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C12" t="s">
         <v>125</v>
@@ -6102,7 +6140,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C13" t="s">
         <v>126</v>
@@ -6113,7 +6151,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C14" t="s">
         <v>127</v>
@@ -6124,7 +6162,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C15" t="s">
         <v>128</v>
@@ -6135,7 +6173,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C16" t="s">
         <v>129</v>
@@ -6146,7 +6184,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C17" t="s">
         <v>130</v>
@@ -6157,7 +6195,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>777</v>
       </c>
       <c r="C18" t="s">
         <v>131</v>
@@ -6168,7 +6206,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>777</v>
       </c>
       <c r="C19" t="s">
         <v>132</v>
@@ -6179,7 +6217,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>777</v>
       </c>
       <c r="C20" t="s">
         <v>133</v>
@@ -6190,7 +6228,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>777</v>
       </c>
       <c r="C21" t="s">
         <v>134</v>
@@ -6201,7 +6239,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C22" t="s">
         <v>135</v>
@@ -6212,7 +6250,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C23" t="s">
         <v>136</v>
@@ -6271,7 +6309,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C6" t="s">
         <v>103</v>
@@ -6282,7 +6320,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C7" t="s">
         <v>104</v>
@@ -6293,7 +6331,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C8" t="s">
         <v>105</v>
@@ -6304,7 +6342,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C9" t="s">
         <v>106</v>
@@ -6315,7 +6353,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C10" t="s">
         <v>107</v>
@@ -6326,7 +6364,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C11" t="s">
         <v>108</v>
@@ -6337,7 +6375,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C12" t="s">
         <v>109</v>
@@ -6348,7 +6386,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C13" t="s">
         <v>110</v>
@@ -6359,7 +6397,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C14" t="s">
         <v>111</v>
@@ -6370,7 +6408,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C15" t="s">
         <v>112</v>
@@ -6381,7 +6419,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C16" t="s">
         <v>113</v>
@@ -6392,7 +6430,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C17" t="s">
         <v>114</v>
@@ -6403,7 +6441,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C18" t="s">
         <v>115</v>
@@ -6414,7 +6452,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>778</v>
       </c>
       <c r="C19" t="s">
         <v>116</v>
@@ -6425,7 +6463,7 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C20" t="s">
         <v>117</v>
@@ -6436,7 +6474,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>778</v>
       </c>
       <c r="C21" t="s">
         <v>118</v>
@@ -6447,7 +6485,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>778</v>
       </c>
       <c r="C22" t="s">
         <v>119</v>
@@ -6506,7 +6544,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C6" t="s">
         <v>78</v>
@@ -6517,7 +6555,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C7" t="s">
         <v>79</v>
@@ -6528,7 +6566,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C8" t="s">
         <v>80</v>
@@ -6539,7 +6577,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C9" t="s">
         <v>81</v>
@@ -6550,7 +6588,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C10" t="s">
         <v>82</v>
@@ -6561,7 +6599,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C11" t="s">
         <v>83</v>
@@ -6572,7 +6610,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C12" t="s">
         <v>84</v>
@@ -6583,7 +6621,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C13" t="s">
         <v>85</v>
@@ -6594,7 +6632,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C14" t="s">
         <v>86</v>
@@ -6605,7 +6643,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C15" t="s">
         <v>87</v>
@@ -6616,7 +6654,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C16" t="s">
         <v>88</v>
@@ -6627,7 +6665,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C17" t="s">
         <v>89</v>
@@ -6638,7 +6676,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C18" t="s">
         <v>90</v>
@@ -6649,7 +6687,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C19" t="s">
         <v>91</v>
@@ -6660,7 +6698,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C20" t="s">
         <v>92</v>
@@ -6671,7 +6709,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C21" t="s">
         <v>93</v>
@@ -6682,7 +6720,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C22" t="s">
         <v>94</v>
@@ -6693,7 +6731,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C23" t="s">
         <v>95</v>
@@ -6704,7 +6742,7 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C24" t="s">
         <v>96</v>
@@ -6715,7 +6753,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
+        <v>776</v>
       </c>
       <c r="C25" t="s">
         <v>97</v>
@@ -6726,7 +6764,7 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>776</v>
       </c>
       <c r="C26" t="s">
         <v>98</v>
@@ -6737,7 +6775,7 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>776</v>
       </c>
       <c r="C27" t="s">
         <v>99</v>
@@ -6748,7 +6786,7 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C28" t="s">
         <v>100</v>
@@ -6759,7 +6797,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>2</v>
+        <v>774</v>
       </c>
       <c r="C29" t="s">
         <v>101</v>
@@ -6770,7 +6808,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>776</v>
       </c>
       <c r="C30" t="s">
         <v>102</v>
@@ -6829,7 +6867,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>782</v>
       </c>
       <c r="C6" t="s">
         <v>43</v>
@@ -6840,7 +6878,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>782</v>
       </c>
       <c r="C7" t="s">
         <v>44</v>
@@ -6851,7 +6889,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>782</v>
       </c>
       <c r="C8" t="s">
         <v>45</v>
@@ -6862,7 +6900,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>782</v>
       </c>
       <c r="C9" t="s">
         <v>46</v>
@@ -6873,7 +6911,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>782</v>
       </c>
       <c r="C10" t="s">
         <v>47</v>
@@ -6884,7 +6922,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>782</v>
       </c>
       <c r="C11" t="s">
         <v>48</v>
@@ -6895,7 +6933,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>782</v>
       </c>
       <c r="C12" t="s">
         <v>49</v>
@@ -6906,7 +6944,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>782</v>
       </c>
       <c r="C13" t="s">
         <v>50</v>
@@ -6917,7 +6955,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>782</v>
       </c>
       <c r="C14" t="s">
         <v>51</v>
@@ -6928,7 +6966,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>782</v>
       </c>
       <c r="C15" t="s">
         <v>52</v>
@@ -6939,7 +6977,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>782</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>28</v>
@@ -6950,7 +6988,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>782</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>29</v>
@@ -6961,7 +6999,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>782</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>30</v>
@@ -6972,7 +7010,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>782</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>31</v>
@@ -6983,7 +7021,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>782</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>32</v>
@@ -6994,7 +7032,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>782</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>33</v>
@@ -7005,7 +7043,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>781</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>34</v>
@@ -7016,7 +7054,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>781</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>35</v>
@@ -7027,7 +7065,7 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>781</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>36</v>
@@ -7038,7 +7076,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
+        <v>781</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>37</v>
@@ -7049,7 +7087,7 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>781</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>38</v>
@@ -7060,7 +7098,7 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>781</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>39</v>
@@ -7071,7 +7109,7 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>3</v>
+        <v>781</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>40</v>
@@ -7082,7 +7120,7 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>781</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>41</v>
@@ -7093,7 +7131,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>781</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>42</v>
@@ -7146,7 +7184,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B6" t="s">
         <v>54</v>
@@ -7154,7 +7192,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B7" t="s">
         <v>55</v>
@@ -7162,7 +7200,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B8" t="s">
         <v>53</v>
@@ -7170,7 +7208,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B9" t="s">
         <v>56</v>
@@ -7178,7 +7216,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B10" t="s">
         <v>57</v>
@@ -7186,7 +7224,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B11" t="s">
         <v>58</v>
@@ -7194,7 +7232,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B12" t="s">
         <v>59</v>
@@ -7202,7 +7240,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B13" t="s">
         <v>60</v>
@@ -7210,7 +7248,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B14" t="s">
         <v>61</v>
@@ -7218,7 +7256,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B15" t="s">
         <v>62</v>
@@ -7226,7 +7264,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B16" t="s">
         <v>63</v>
@@ -7234,7 +7272,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B17" t="s">
         <v>64</v>
@@ -7242,7 +7280,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B18" t="s">
         <v>65</v>
@@ -7250,7 +7288,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B19" t="s">
         <v>66</v>
@@ -7258,7 +7296,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B20" t="s">
         <v>67</v>
@@ -7266,7 +7304,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B21" t="s">
         <v>68</v>
@@ -7274,7 +7312,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B22" t="s">
         <v>69</v>
@@ -7282,7 +7320,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B23" t="s">
         <v>70</v>
@@ -7290,7 +7328,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B24" t="s">
         <v>71</v>
@@ -7298,7 +7336,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>779</v>
       </c>
       <c r="B25" t="s">
         <v>72</v>
@@ -7306,7 +7344,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>3</v>
+        <v>780</v>
       </c>
       <c r="B26" t="s">
         <v>73</v>
@@ -7314,7 +7352,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>3</v>
+        <v>780</v>
       </c>
       <c r="B27" t="s">
         <v>74</v>
@@ -7322,7 +7360,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>3</v>
+        <v>780</v>
       </c>
       <c r="B28" t="s">
         <v>75</v>
@@ -7330,7 +7368,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>3</v>
+        <v>780</v>
       </c>
       <c r="B29" t="s">
         <v>76</v>
@@ -7338,7 +7376,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>3</v>
+        <v>780</v>
       </c>
       <c r="B30" t="s">
         <v>77</v>
@@ -8808,7 +8846,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{021C946B-314F-4475-9B2D-C8EA00D9D464}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:B56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -9314,7 +9354,7 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>3</v>
+        <v>773</v>
       </c>
       <c r="C48" t="s">
         <v>500</v>
@@ -9325,7 +9365,7 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>773</v>
       </c>
       <c r="C49" t="s">
         <v>501</v>
@@ -9336,7 +9376,7 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>3</v>
+        <v>773</v>
       </c>
       <c r="C50" t="s">
         <v>502</v>
@@ -9347,7 +9387,7 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>3</v>
+        <v>773</v>
       </c>
       <c r="C51" t="s">
         <v>503</v>
@@ -9358,7 +9398,7 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>3</v>
+        <v>773</v>
       </c>
       <c r="C52" t="s">
         <v>504</v>
@@ -9369,7 +9409,7 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>3</v>
+        <v>773</v>
       </c>
       <c r="C53" t="s">
         <v>405</v>
@@ -9380,7 +9420,7 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>3</v>
+        <v>773</v>
       </c>
       <c r="C54" t="s">
         <v>505</v>
@@ -9391,7 +9431,7 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>3</v>
+        <v>773</v>
       </c>
       <c r="C55" t="s">
         <v>506</v>
@@ -9402,7 +9442,7 @@
         <v>760</v>
       </c>
       <c r="B56" t="s">
-        <v>3</v>
+        <v>773</v>
       </c>
       <c r="C56" t="s">
         <v>507</v>

</xml_diff>

<commit_message>
change button text, hover information for button, add special word colour to own it deck
</commit_message>
<xml_diff>
--- a/data/WNRS.xlsx
+++ b/data/WNRS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KayJan\test-app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AFA170-018D-4B86-B28F-96E82F8FBB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03587DC4-1623-4F51-82C8-F0B071A0FE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="-13710" windowWidth="14745" windowHeight="11685" tabRatio="829" firstSheet="9" activeTab="12" xr2:uid="{35520F66-FEA5-4575-927A-C3FC8E8C1344}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="829" firstSheet="6" activeTab="8" xr2:uid="{35520F66-FEA5-4575-927A-C3FC8E8C1344}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Deck" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="787">
   <si>
     <t>Card</t>
   </si>
@@ -2027,45 +2027,6 @@
     <t>Wild Card Write down the top 3 things\n you're most grateful for in\n your partner. 30 seconds.\n Compare.</t>
   </si>
   <si>
-    <t>What part(s) of yourself\n have you been minimizing that\n you're ready to finally own?\n Permission to (own it).</t>
-  </si>
-  <si>
-    <t>Who do you feel misunderstood by? What do you wish they would come to understand?</t>
-  </si>
-  <si>
-    <t>What lesson in love\n took you the longest\n to learn?</t>
-  </si>
-  <si>
-    <t>What act of kindness\n from a stranger will\n you never forget?</t>
-  </si>
-  <si>
-    <t>What has your heart\n been telling you that\n you've been ignoring?</t>
-  </si>
-  <si>
-    <t>What have you not forgiven that hurts you the most?</t>
-  </si>
-  <si>
-    <t>What have you envied\n in the past that you\n can laugh at now?</t>
-  </si>
-  <si>
-    <t>What door are you most\n grateful for closing that\n felt like the end of\n the world at the time? What\n did it open for you?</t>
-  </si>
-  <si>
-    <t>What do you wish\n you had the courage\n to do? To say?</t>
-  </si>
-  <si>
-    <t>What (blame have you been placing on someone else that you can take some accountability for?</t>
-  </si>
-  <si>
-    <t>Wild Card Set an intention for\n today, this month and\n this year. Write it out.</t>
-  </si>
-  <si>
-    <t>Wild Card Spend at least 5 minutes in nature today. Be still and observe. What did you notice?</t>
-  </si>
-  <si>
-    <t>Wild Card Write down 3 things\n you're most grateful for\n in this present moment.\n Big or small.</t>
-  </si>
-  <si>
     <t>Just by looking at me,\n what would you think\n I do for a living?</t>
   </si>
   <si>
@@ -2289,45 +2250,6 @@
   </si>
   <si>
     <t>Wild Card Finish the sentence:\n Thank you for _________.\n Both players.</t>
-  </si>
-  <si>
-    <t>When was the last time you felt complete zen? Who were you with? Where were you? What were you doing?</t>
-  </si>
-  <si>
-    <t>What is your x-factor?\n Permission to brag.</t>
-  </si>
-  <si>
-    <t>Who is a woman in your life that inspires you to be a better person? Why does she come to mind? (Send her a thank you)</t>
-  </si>
-  <si>
-    <t>What still feels vulnerable in your life? What does owning it look like for you?</t>
-  </si>
-  <si>
-    <t>Who from your past would you want to reunite with? What would you ask them?</t>
-  </si>
-  <si>
-    <t>What's the hardest truth\n you've had to own\n this past year? What has\n owning it taught you?</t>
-  </si>
-  <si>
-    <t>How has your definition of success evolved over time? What is your definition of it today? Get specific.</t>
-  </si>
-  <si>
-    <t>Who in your life do you want to build a deeper relationship with? (Be direct and tell them)</t>
-  </si>
-  <si>
-    <t>What question have you\n avoided asking someone? What\n question have you avoided\n asking yourself?</t>
-  </si>
-  <si>
-    <t>What area of your life have you made the most progress in recently? Get specific. Take a moment to congratulate yourself.</t>
-  </si>
-  <si>
-    <t>What has brought you the most unexpected joy recently?</t>
-  </si>
-  <si>
-    <t>What have you become\n newly aware of within\n yourself recently?\n Get specific.</t>
-  </si>
-  <si>
-    <t>How would you describe\n your relationship with yourself\n in one word?</t>
   </si>
   <si>
     <t>-</t>
@@ -2475,6 +2397,93 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>When was the last time you felt complete [#af2637](zen)? Who were you with? Where were you? What were you doing?</t>
+  </si>
+  <si>
+    <t>How would you describe\n your relationship with [#d0af3a](yourself)\n in one word?</t>
+  </si>
+  <si>
+    <t>What is your [#275835](x-factor)?\n Permission to brag.</t>
+  </si>
+  <si>
+    <t>Who is a [#c66532](woman) in your life that inspires you to be a better person? Why does she come to mind? (Send her a thank you)</t>
+  </si>
+  <si>
+    <t>What still feels [#c97986](vulnerable) in your life? What does owning it look like for you?</t>
+  </si>
+  <si>
+    <t>Who from your past would you want to [#5f86b5](reunite) with? What would you ask them?</t>
+  </si>
+  <si>
+    <t>What's the hardest [#275835](truth)\n you've had to own\n this past year? What has\n owning it taught you?</t>
+  </si>
+  <si>
+    <t>How has your definition of [#d0af3a](success) evolved over time? What is your definition of it today? Get specific.</t>
+  </si>
+  <si>
+    <t>Who in your life do you want to build a deeper [#af2637](relationship) with? (Be direct and tell them)</t>
+  </si>
+  <si>
+    <t>What [#5f86b5](question) have you\n avoided asking someone? What\n question have you avoided\n asking yourself?</t>
+  </si>
+  <si>
+    <t>What area of your life have you made the most [#c97986](progress) in recently? Get specific. Take a moment to congratulate yourself.</t>
+  </si>
+  <si>
+    <t>What part(s) of yourself\n have you been minimizing that\n you're ready to finally own?\n Permission to [#c97986](own it).</t>
+  </si>
+  <si>
+    <t>Who do you feel [#d0af3a](misunderstood) by? What do you wish they would come to understand?</t>
+  </si>
+  <si>
+    <t>What lesson in [#275835](love)\n took you the longest\n to learn?</t>
+  </si>
+  <si>
+    <t>What act of [#c66532](kindness)\n from a stranger will\n you never forget?</t>
+  </si>
+  <si>
+    <t>What has brought you the most unexpected [#c97986](joy) recently?</t>
+  </si>
+  <si>
+    <t>What has your [#af2637](heart)\n been telling you that\n you've been ignoring?</t>
+  </si>
+  <si>
+    <t>What have you not [#d0af3a](forgiven) that hurts you the most?</t>
+  </si>
+  <si>
+    <t>What have you [#c66532](envied)\n in the past that you\n can laugh at now?</t>
+  </si>
+  <si>
+    <t>What [#c97986](door) are you most\n grateful for closing that\n felt like the end of\n the world at the time? What\n did it open for you?</t>
+  </si>
+  <si>
+    <t>What do you wish\n you had the [#af2637](courage)\n to do? To say?</t>
+  </si>
+  <si>
+    <t>What [#5f86b5](blame) have you been placing on someone else that you can take some accountability for?</t>
+  </si>
+  <si>
+    <t>What have you become\n newly [#d0af3a](aware) of within\n yourself recently?\n Get specific.</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>Wild Card Set an intention for\n today, this month and\n this year. Write it out.</t>
+  </si>
+  <si>
+    <t>Wild Card Spend at least 5 minutes in nature today. Be still and observe. What did you notice?</t>
+  </si>
+  <si>
+    <t>Wild Card Write down 3 things\n you're most grateful for\n in this present moment.\n Big or small.</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S2</t>
   </si>
 </sst>
 </file>
@@ -2855,7 +2864,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>761</v>
+        <v>735</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -4529,7 +4538,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>760</v>
+        <v>734</v>
       </c>
       <c r="B156" t="s">
         <v>3</v>
@@ -4566,7 +4575,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>766</v>
+        <v>740</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -5208,7 +5217,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>767</v>
+        <v>741</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -5235,7 +5244,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C6" t="s">
         <v>579</v>
@@ -5246,7 +5255,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C7" t="s">
         <v>580</v>
@@ -5257,7 +5266,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>775</v>
+        <v>749</v>
       </c>
       <c r="C8" t="s">
         <v>581</v>
@@ -5268,7 +5277,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C9" t="s">
         <v>582</v>
@@ -5279,7 +5288,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C10" t="s">
         <v>583</v>
@@ -5290,7 +5299,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C11" t="s">
         <v>584</v>
@@ -5301,7 +5310,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C12" t="s">
         <v>585</v>
@@ -5312,7 +5321,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C13" t="s">
         <v>586</v>
@@ -5323,7 +5332,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C14" t="s">
         <v>587</v>
@@ -5334,7 +5343,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C15" t="s">
         <v>588</v>
@@ -5345,7 +5354,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C16" t="s">
         <v>589</v>
@@ -5356,7 +5365,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C17" t="s">
         <v>590</v>
@@ -5367,7 +5376,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C18" t="s">
         <v>591</v>
@@ -5378,7 +5387,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C19" t="s">
         <v>592</v>
@@ -5389,7 +5398,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C20" t="s">
         <v>593</v>
@@ -5400,7 +5409,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C21" t="s">
         <v>594</v>
@@ -5411,7 +5420,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C22" t="s">
         <v>595</v>
@@ -5422,7 +5431,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C23" t="s">
         <v>596</v>
@@ -5433,7 +5442,7 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C24" t="s">
         <v>597</v>
@@ -5444,7 +5453,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C25" t="s">
         <v>598</v>
@@ -5455,7 +5464,7 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>775</v>
+        <v>749</v>
       </c>
       <c r="C26" t="s">
         <v>599</v>
@@ -5466,7 +5475,7 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C27" t="s">
         <v>600</v>
@@ -5477,7 +5486,7 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C28" t="s">
         <v>601</v>
@@ -5488,7 +5497,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C29" t="s">
         <v>602</v>
@@ -5499,7 +5508,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>775</v>
+        <v>749</v>
       </c>
       <c r="C30" t="s">
         <v>603</v>
@@ -5532,7 +5541,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>759</v>
+        <v>733</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -5754,7 +5763,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>760</v>
+        <v>734</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
@@ -5772,7 +5781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941E7727-1D5F-48BE-8AE3-2119045C4067}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -5789,7 +5798,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>769</v>
+        <v>743</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -5810,7 +5819,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B6" t="s">
         <v>137</v>
@@ -5818,7 +5827,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B7" t="s">
         <v>138</v>
@@ -5826,7 +5835,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B8" t="s">
         <v>139</v>
@@ -5834,7 +5843,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B9" t="s">
         <v>140</v>
@@ -5842,7 +5851,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B10" t="s">
         <v>141</v>
@@ -5850,7 +5859,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B11" t="s">
         <v>142</v>
@@ -5858,7 +5867,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B12" t="s">
         <v>143</v>
@@ -5866,7 +5875,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B13" t="s">
         <v>144</v>
@@ -5874,7 +5883,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B14" t="s">
         <v>145</v>
@@ -5882,7 +5891,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B15" t="s">
         <v>146</v>
@@ -5890,7 +5899,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B16" t="s">
         <v>147</v>
@@ -5898,7 +5907,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B17" t="s">
         <v>148</v>
@@ -5906,7 +5915,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B18" t="s">
         <v>149</v>
@@ -5914,7 +5923,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B19" t="s">
         <v>150</v>
@@ -5922,7 +5931,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B20" t="s">
         <v>151</v>
@@ -5930,7 +5939,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B21" t="s">
         <v>152</v>
@@ -5938,7 +5947,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B22" t="s">
         <v>153</v>
@@ -5946,7 +5955,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B23" t="s">
         <v>154</v>
@@ -5954,7 +5963,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B24" t="s">
         <v>155</v>
@@ -5962,7 +5971,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B25" t="s">
         <v>156</v>
@@ -5970,7 +5979,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B26" t="s">
         <v>157</v>
@@ -5978,7 +5987,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B27" t="s">
         <v>158</v>
@@ -5986,7 +5995,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="B28" t="s">
         <v>159</v>
@@ -5994,7 +6003,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>783</v>
+        <v>757</v>
       </c>
       <c r="B29" t="s">
         <v>160</v>
@@ -6002,7 +6011,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>783</v>
+        <v>757</v>
       </c>
       <c r="B30" t="s">
         <v>161</v>
@@ -6036,7 +6045,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>759</v>
+        <v>733</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -6063,7 +6072,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C6" t="s">
         <v>120</v>
@@ -6074,7 +6083,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C7" t="s">
         <v>121</v>
@@ -6085,7 +6094,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C8" t="s">
         <v>91</v>
@@ -6096,7 +6105,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C9" t="s">
         <v>122</v>
@@ -6107,7 +6116,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C10" t="s">
         <v>123</v>
@@ -6118,7 +6127,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C11" t="s">
         <v>124</v>
@@ -6129,7 +6138,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C12" t="s">
         <v>125</v>
@@ -6140,7 +6149,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C13" t="s">
         <v>126</v>
@@ -6151,7 +6160,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C14" t="s">
         <v>127</v>
@@ -6162,7 +6171,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C15" t="s">
         <v>128</v>
@@ -6173,7 +6182,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C16" t="s">
         <v>129</v>
@@ -6184,7 +6193,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C17" t="s">
         <v>130</v>
@@ -6195,7 +6204,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>777</v>
+        <v>751</v>
       </c>
       <c r="C18" t="s">
         <v>131</v>
@@ -6206,7 +6215,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>777</v>
+        <v>751</v>
       </c>
       <c r="C19" t="s">
         <v>132</v>
@@ -6217,7 +6226,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>777</v>
+        <v>751</v>
       </c>
       <c r="C20" t="s">
         <v>133</v>
@@ -6228,7 +6237,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>777</v>
+        <v>751</v>
       </c>
       <c r="C21" t="s">
         <v>134</v>
@@ -6239,7 +6248,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C22" t="s">
         <v>135</v>
@@ -6250,7 +6259,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C23" t="s">
         <v>136</v>
@@ -6282,7 +6291,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>759</v>
+        <v>733</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -6309,7 +6318,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C6" t="s">
         <v>103</v>
@@ -6320,7 +6329,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C7" t="s">
         <v>104</v>
@@ -6331,7 +6340,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C8" t="s">
         <v>105</v>
@@ -6342,7 +6351,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C9" t="s">
         <v>106</v>
@@ -6353,7 +6362,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C10" t="s">
         <v>107</v>
@@ -6364,7 +6373,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C11" t="s">
         <v>108</v>
@@ -6375,7 +6384,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C12" t="s">
         <v>109</v>
@@ -6386,7 +6395,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C13" t="s">
         <v>110</v>
@@ -6397,7 +6406,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C14" t="s">
         <v>111</v>
@@ -6408,7 +6417,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C15" t="s">
         <v>112</v>
@@ -6419,7 +6428,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C16" t="s">
         <v>113</v>
@@ -6430,7 +6439,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C17" t="s">
         <v>114</v>
@@ -6441,7 +6450,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C18" t="s">
         <v>115</v>
@@ -6452,7 +6461,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>778</v>
+        <v>752</v>
       </c>
       <c r="C19" t="s">
         <v>116</v>
@@ -6463,7 +6472,7 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C20" t="s">
         <v>117</v>
@@ -6474,7 +6483,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>778</v>
+        <v>752</v>
       </c>
       <c r="C21" t="s">
         <v>118</v>
@@ -6485,7 +6494,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>778</v>
+        <v>752</v>
       </c>
       <c r="C22" t="s">
         <v>119</v>
@@ -6517,7 +6526,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>759</v>
+        <v>733</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -6544,7 +6553,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C6" t="s">
         <v>78</v>
@@ -6555,7 +6564,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C7" t="s">
         <v>79</v>
@@ -6566,7 +6575,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C8" t="s">
         <v>80</v>
@@ -6577,7 +6586,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C9" t="s">
         <v>81</v>
@@ -6588,7 +6597,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C10" t="s">
         <v>82</v>
@@ -6599,7 +6608,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C11" t="s">
         <v>83</v>
@@ -6610,7 +6619,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C12" t="s">
         <v>84</v>
@@ -6621,7 +6630,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C13" t="s">
         <v>85</v>
@@ -6632,7 +6641,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C14" t="s">
         <v>86</v>
@@ -6643,7 +6652,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C15" t="s">
         <v>87</v>
@@ -6654,7 +6663,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C16" t="s">
         <v>88</v>
@@ -6665,7 +6674,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C17" t="s">
         <v>89</v>
@@ -6676,7 +6685,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C18" t="s">
         <v>90</v>
@@ -6687,7 +6696,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C19" t="s">
         <v>91</v>
@@ -6698,7 +6707,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C20" t="s">
         <v>92</v>
@@ -6709,7 +6718,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C21" t="s">
         <v>93</v>
@@ -6720,7 +6729,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C22" t="s">
         <v>94</v>
@@ -6731,7 +6740,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C23" t="s">
         <v>95</v>
@@ -6742,7 +6751,7 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C24" t="s">
         <v>96</v>
@@ -6753,7 +6762,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>776</v>
+        <v>750</v>
       </c>
       <c r="C25" t="s">
         <v>97</v>
@@ -6764,7 +6773,7 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>776</v>
+        <v>750</v>
       </c>
       <c r="C26" t="s">
         <v>98</v>
@@ -6775,7 +6784,7 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>776</v>
+        <v>750</v>
       </c>
       <c r="C27" t="s">
         <v>99</v>
@@ -6786,7 +6795,7 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C28" t="s">
         <v>100</v>
@@ -6797,7 +6806,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
       <c r="C29" t="s">
         <v>101</v>
@@ -6808,7 +6817,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>776</v>
+        <v>750</v>
       </c>
       <c r="C30" t="s">
         <v>102</v>
@@ -6840,7 +6849,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>759</v>
+        <v>733</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -6867,7 +6876,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>782</v>
+        <v>756</v>
       </c>
       <c r="C6" t="s">
         <v>43</v>
@@ -6878,7 +6887,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>782</v>
+        <v>756</v>
       </c>
       <c r="C7" t="s">
         <v>44</v>
@@ -6889,7 +6898,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>782</v>
+        <v>756</v>
       </c>
       <c r="C8" t="s">
         <v>45</v>
@@ -6900,7 +6909,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>782</v>
+        <v>756</v>
       </c>
       <c r="C9" t="s">
         <v>46</v>
@@ -6911,7 +6920,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>782</v>
+        <v>756</v>
       </c>
       <c r="C10" t="s">
         <v>47</v>
@@ -6922,7 +6931,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>782</v>
+        <v>756</v>
       </c>
       <c r="C11" t="s">
         <v>48</v>
@@ -6933,7 +6942,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>782</v>
+        <v>756</v>
       </c>
       <c r="C12" t="s">
         <v>49</v>
@@ -6944,7 +6953,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>782</v>
+        <v>756</v>
       </c>
       <c r="C13" t="s">
         <v>50</v>
@@ -6955,7 +6964,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>782</v>
+        <v>756</v>
       </c>
       <c r="C14" t="s">
         <v>51</v>
@@ -6966,7 +6975,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>782</v>
+        <v>756</v>
       </c>
       <c r="C15" t="s">
         <v>52</v>
@@ -6977,7 +6986,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>782</v>
+        <v>756</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>28</v>
@@ -6988,7 +6997,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>782</v>
+        <v>756</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>29</v>
@@ -6999,7 +7008,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>782</v>
+        <v>756</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>30</v>
@@ -7010,7 +7019,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>782</v>
+        <v>756</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>31</v>
@@ -7021,7 +7030,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>782</v>
+        <v>756</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>32</v>
@@ -7032,7 +7041,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>782</v>
+        <v>756</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>33</v>
@@ -7043,7 +7052,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>781</v>
+        <v>755</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>34</v>
@@ -7054,7 +7063,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>781</v>
+        <v>755</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>35</v>
@@ -7065,7 +7074,7 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>781</v>
+        <v>755</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>36</v>
@@ -7076,7 +7085,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>781</v>
+        <v>755</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>37</v>
@@ -7087,7 +7096,7 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>781</v>
+        <v>755</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>38</v>
@@ -7098,7 +7107,7 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>781</v>
+        <v>755</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>39</v>
@@ -7109,7 +7118,7 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>781</v>
+        <v>755</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>40</v>
@@ -7120,7 +7129,7 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>781</v>
+        <v>755</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>41</v>
@@ -7131,7 +7140,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>781</v>
+        <v>755</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>42</v>
@@ -7163,7 +7172,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>768</v>
+        <v>742</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -7184,7 +7193,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B6" t="s">
         <v>54</v>
@@ -7192,7 +7201,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B7" t="s">
         <v>55</v>
@@ -7200,7 +7209,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B8" t="s">
         <v>53</v>
@@ -7208,7 +7217,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B9" t="s">
         <v>56</v>
@@ -7216,7 +7225,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B10" t="s">
         <v>57</v>
@@ -7224,7 +7233,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B11" t="s">
         <v>58</v>
@@ -7232,7 +7241,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B12" t="s">
         <v>59</v>
@@ -7240,7 +7249,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B13" t="s">
         <v>60</v>
@@ -7248,7 +7257,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B14" t="s">
         <v>61</v>
@@ -7256,7 +7265,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B15" t="s">
         <v>62</v>
@@ -7264,7 +7273,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B16" t="s">
         <v>63</v>
@@ -7272,7 +7281,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B17" t="s">
         <v>64</v>
@@ -7280,7 +7289,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B18" t="s">
         <v>65</v>
@@ -7288,7 +7297,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B19" t="s">
         <v>66</v>
@@ -7296,7 +7305,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B20" t="s">
         <v>67</v>
@@ -7304,7 +7313,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B21" t="s">
         <v>68</v>
@@ -7312,7 +7321,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B22" t="s">
         <v>69</v>
@@ -7320,7 +7329,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B23" t="s">
         <v>70</v>
@@ -7328,7 +7337,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B24" t="s">
         <v>71</v>
@@ -7336,7 +7345,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>779</v>
+        <v>753</v>
       </c>
       <c r="B25" t="s">
         <v>72</v>
@@ -7344,7 +7353,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>780</v>
+        <v>754</v>
       </c>
       <c r="B26" t="s">
         <v>73</v>
@@ -7352,7 +7361,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>780</v>
+        <v>754</v>
       </c>
       <c r="B27" t="s">
         <v>74</v>
@@ -7360,7 +7369,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>780</v>
+        <v>754</v>
       </c>
       <c r="B28" t="s">
         <v>75</v>
@@ -7368,7 +7377,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>780</v>
+        <v>754</v>
       </c>
       <c r="B29" t="s">
         <v>76</v>
@@ -7376,7 +7385,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>780</v>
+        <v>754</v>
       </c>
       <c r="B30" t="s">
         <v>77</v>
@@ -7408,7 +7417,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>762</v>
+        <v>736</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -7938,7 +7947,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>760</v>
+        <v>734</v>
       </c>
       <c r="B52" t="s">
         <v>3</v>
@@ -7973,7 +7982,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>763</v>
+        <v>737</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -8418,7 +8427,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>770</v>
+        <v>744</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -8865,7 +8874,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>771</v>
+        <v>745</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -8873,7 +8882,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>772</v>
+        <v>746</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -9354,7 +9363,7 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>773</v>
+        <v>747</v>
       </c>
       <c r="C48" t="s">
         <v>500</v>
@@ -9365,7 +9374,7 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>773</v>
+        <v>747</v>
       </c>
       <c r="C49" t="s">
         <v>501</v>
@@ -9376,7 +9385,7 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>773</v>
+        <v>747</v>
       </c>
       <c r="C50" t="s">
         <v>502</v>
@@ -9387,7 +9396,7 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>773</v>
+        <v>747</v>
       </c>
       <c r="C51" t="s">
         <v>503</v>
@@ -9398,7 +9407,7 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>773</v>
+        <v>747</v>
       </c>
       <c r="C52" t="s">
         <v>504</v>
@@ -9409,7 +9418,7 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>773</v>
+        <v>747</v>
       </c>
       <c r="C53" t="s">
         <v>405</v>
@@ -9420,7 +9429,7 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>773</v>
+        <v>747</v>
       </c>
       <c r="C54" t="s">
         <v>505</v>
@@ -9431,7 +9440,7 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>773</v>
+        <v>747</v>
       </c>
       <c r="C55" t="s">
         <v>506</v>
@@ -9439,10 +9448,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>760</v>
+        <v>734</v>
       </c>
       <c r="B56" t="s">
-        <v>773</v>
+        <v>747</v>
       </c>
       <c r="C56" t="s">
         <v>507</v>
@@ -9474,7 +9483,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>759</v>
+        <v>733</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -9935,7 +9944,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>764</v>
+        <v>738</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -9965,7 +9974,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -9976,7 +9985,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>672</v>
+        <v>659</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -9987,7 +9996,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>673</v>
+        <v>660</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -9998,7 +10007,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>674</v>
+        <v>661</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -10009,7 +10018,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>675</v>
+        <v>662</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -10020,7 +10029,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>676</v>
+        <v>663</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -10031,7 +10040,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>677</v>
+        <v>664</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -10042,7 +10051,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>678</v>
+        <v>665</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -10053,7 +10062,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>679</v>
+        <v>666</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -10064,7 +10073,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>680</v>
+        <v>667</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -10075,7 +10084,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>681</v>
+        <v>668</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -10086,7 +10095,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>682</v>
+        <v>669</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -10097,7 +10106,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>683</v>
+        <v>670</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -10108,7 +10117,7 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>684</v>
+        <v>671</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -10119,7 +10128,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>685</v>
+        <v>672</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -10130,7 +10139,7 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>686</v>
+        <v>673</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -10141,7 +10150,7 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>687</v>
+        <v>674</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -10152,7 +10161,7 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>688</v>
+        <v>675</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -10163,7 +10172,7 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>689</v>
+        <v>676</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -10174,7 +10183,7 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>690</v>
+        <v>677</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -10185,7 +10194,7 @@
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>691</v>
+        <v>678</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -10196,7 +10205,7 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>692</v>
+        <v>679</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -10207,7 +10216,7 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>693</v>
+        <v>680</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -10218,7 +10227,7 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>694</v>
+        <v>681</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -10229,7 +10238,7 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>695</v>
+        <v>682</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -10240,7 +10249,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>696</v>
+        <v>683</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -10251,7 +10260,7 @@
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>697</v>
+        <v>684</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -10262,7 +10271,7 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>698</v>
+        <v>685</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -10273,7 +10282,7 @@
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>699</v>
+        <v>686</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -10284,7 +10293,7 @@
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>700</v>
+        <v>687</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -10295,7 +10304,7 @@
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>701</v>
+        <v>688</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -10306,7 +10315,7 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>702</v>
+        <v>689</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -10317,7 +10326,7 @@
         <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>703</v>
+        <v>690</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -10328,7 +10337,7 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>704</v>
+        <v>691</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -10339,7 +10348,7 @@
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>705</v>
+        <v>692</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -10350,7 +10359,7 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>706</v>
+        <v>693</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -10361,7 +10370,7 @@
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>707</v>
+        <v>694</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -10372,7 +10381,7 @@
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>708</v>
+        <v>695</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -10383,7 +10392,7 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>709</v>
+        <v>696</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -10394,7 +10403,7 @@
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>710</v>
+        <v>697</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -10405,7 +10414,7 @@
         <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>711</v>
+        <v>698</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -10416,7 +10425,7 @@
         <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>712</v>
+        <v>699</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -10427,7 +10436,7 @@
         <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>713</v>
+        <v>700</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -10438,7 +10447,7 @@
         <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>714</v>
+        <v>701</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -10449,7 +10458,7 @@
         <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>715</v>
+        <v>702</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -10460,7 +10469,7 @@
         <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>716</v>
+        <v>703</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -10471,7 +10480,7 @@
         <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>717</v>
+        <v>704</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -10482,7 +10491,7 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>718</v>
+        <v>705</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -10493,7 +10502,7 @@
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>719</v>
+        <v>706</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -10504,7 +10513,7 @@
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>720</v>
+        <v>707</v>
       </c>
     </row>
   </sheetData>
@@ -10533,7 +10542,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>759</v>
+        <v>733</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -10563,7 +10572,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>721</v>
+        <v>708</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -10574,7 +10583,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>722</v>
+        <v>709</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -10585,7 +10594,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>723</v>
+        <v>710</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -10596,7 +10605,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>724</v>
+        <v>711</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -10607,7 +10616,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>725</v>
+        <v>712</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -10618,7 +10627,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>726</v>
+        <v>713</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -10629,7 +10638,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>727</v>
+        <v>714</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -10640,7 +10649,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>728</v>
+        <v>715</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -10651,7 +10660,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>729</v>
+        <v>716</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -10662,7 +10671,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>730</v>
+        <v>717</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -10673,7 +10682,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>731</v>
+        <v>718</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -10684,7 +10693,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>732</v>
+        <v>719</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -10695,7 +10704,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>733</v>
+        <v>720</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -10706,7 +10715,7 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>734</v>
+        <v>721</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -10717,7 +10726,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>735</v>
+        <v>722</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -10728,7 +10737,7 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>736</v>
+        <v>723</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -10739,7 +10748,7 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>737</v>
+        <v>724</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -10750,7 +10759,7 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>738</v>
+        <v>725</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -10761,7 +10770,7 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>739</v>
+        <v>726</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -10772,7 +10781,7 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -10783,7 +10792,7 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>741</v>
+        <v>728</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -10794,7 +10803,7 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>742</v>
+        <v>729</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -10805,7 +10814,7 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>743</v>
+        <v>730</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -10816,7 +10825,7 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>744</v>
+        <v>731</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -10827,7 +10836,7 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>745</v>
+        <v>732</v>
       </c>
     </row>
   </sheetData>
@@ -10839,7 +10848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C622C6D5-49E0-4741-BF5C-484CE802CC93}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -10856,7 +10865,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>765</v>
+        <v>739</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -10877,210 +10886,210 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B6" t="s">
-        <v>746</v>
+        <v>758</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B7" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B8" t="s">
-        <v>747</v>
+        <v>760</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B9" t="s">
-        <v>748</v>
+        <v>761</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B10" t="s">
-        <v>749</v>
+        <v>762</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B11" t="s">
-        <v>750</v>
+        <v>763</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B12" t="s">
-        <v>751</v>
+        <v>764</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B13" t="s">
-        <v>752</v>
+        <v>765</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B14" t="s">
-        <v>753</v>
+        <v>766</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B15" t="s">
-        <v>754</v>
+        <v>767</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B16" t="s">
-        <v>755</v>
+        <v>768</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B17" t="s">
-        <v>658</v>
+        <v>769</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B18" t="s">
-        <v>659</v>
+        <v>770</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B19" t="s">
-        <v>660</v>
+        <v>771</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B20" t="s">
-        <v>661</v>
+        <v>772</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B21" t="s">
-        <v>756</v>
+        <v>773</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B22" t="s">
-        <v>662</v>
+        <v>774</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B23" t="s">
-        <v>663</v>
+        <v>775</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B24" t="s">
-        <v>664</v>
+        <v>776</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B25" t="s">
-        <v>665</v>
+        <v>777</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B26" t="s">
-        <v>666</v>
+        <v>778</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B27" t="s">
-        <v>667</v>
+        <v>779</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="B28" t="s">
-        <v>757</v>
+        <v>780</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>3</v>
+        <v>781</v>
       </c>
       <c r="B29" t="s">
-        <v>668</v>
+        <v>782</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>3</v>
+        <v>786</v>
       </c>
       <c r="B30" t="s">
-        <v>669</v>
+        <v>783</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>3</v>
+        <v>785</v>
       </c>
       <c r="B31" t="s">
-        <v>670</v>
+        <v>784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new pack for WNRS
</commit_message>
<xml_diff>
--- a/data/WNRS.xlsx
+++ b/data/WNRS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KayJan\test-app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4512C437-9245-480C-8415-24B88B053880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EC2D51-3A38-4C9E-A96A-AB1B011CF1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="829" activeTab="4" xr2:uid="{35520F66-FEA5-4575-927A-C3FC8E8C1344}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" tabRatio="829" firstSheet="11" activeTab="18" xr2:uid="{35520F66-FEA5-4575-927A-C3FC8E8C1344}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Deck" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <sheet name="Bumble Date Edition" sheetId="16" r:id="rId16"/>
     <sheet name="Cann Edition" sheetId="17" r:id="rId17"/>
     <sheet name="Valentino Edition" sheetId="18" r:id="rId18"/>
+    <sheet name="Existential Crisis Edition" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="787">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1660" uniqueCount="800">
   <si>
     <t>Card</t>
   </si>
@@ -2473,6 +2474,47 @@
 a friend who is also on their self-love journey. Revisit these questions as often
 as you need. The more we love ourselves, the easier it becomes to give and
 receive love from others. Ready?</t>
+  </si>
+  <si>
+    <t>These are just some thought-provoking questions I encountered online and also
+some daily reminder that might be useful as a timely reminder for yourself.
+Ready?</t>
+  </si>
+  <si>
+    <t>Might cause you to question everything you know</t>
+  </si>
+  <si>
+    <t>Is there someone you’re currently blaming or angry with that you could forgive if tomorrow was your last day on earth?</t>
+  </si>
+  <si>
+    <t>What are you most passionate about?</t>
+  </si>
+  <si>
+    <t>Are you holding back your skills, talents, ideas, or expression so that others won’t feel intimidated?</t>
+  </si>
+  <si>
+    <t>Are you creating your life in a way that feels joyous and inspiring?</t>
+  </si>
+  <si>
+    <t>Do you feel powerful and confident, regardless of your accomplishments or what others think of you?</t>
+  </si>
+  <si>
+    <t>Do you truly love who you authentically are?</t>
+  </si>
+  <si>
+    <t>Am I feeling passionate about my goals and is what I’m doing stimulating me?</t>
+  </si>
+  <si>
+    <t>Am I making choices from a sense of empowerment?</t>
+  </si>
+  <si>
+    <t>Can I let go of something that isn’t working?</t>
+  </si>
+  <si>
+    <t>Can I allow myself to feel fully whatever is coming up?</t>
+  </si>
+  <si>
+    <t>Reminder Remember you have full power over yourself, your reactions, and where you direct your focus.</t>
   </si>
 </sst>
 </file>
@@ -5770,7 +5812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941E7727-1D5F-48BE-8AE3-2119045C4067}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -7387,6 +7429,139 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{711D2D5C-5401-4F25-8002-549E2C45E37A}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>742</v>
+      </c>
+      <c r="B6" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>742</v>
+      </c>
+      <c r="B7" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>742</v>
+      </c>
+      <c r="B8" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>742</v>
+      </c>
+      <c r="B9" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>742</v>
+      </c>
+      <c r="B10" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>742</v>
+      </c>
+      <c r="B11" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>742</v>
+      </c>
+      <c r="B12" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>742</v>
+      </c>
+      <c r="B13" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>742</v>
+      </c>
+      <c r="B14" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>742</v>
+      </c>
+      <c r="B15" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>749</v>
+      </c>
+      <c r="B16" t="s">
+        <v>799</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB7F88C3-FB0C-4B6A-902A-298BB76C9AD4}">
   <dimension ref="A1:C52"/>
@@ -8846,7 +9021,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{021C946B-314F-4475-9B2D-C8EA00D9D464}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="A1:C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>

<commit_message>
Update wnrs card decks, add email helper functions and requirements, add contact me tab, misc css c hanges
</commit_message>
<xml_diff>
--- a/data/WNRS.xlsx
+++ b/data/WNRS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KayJan\test-app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A38CE6-241F-4EF5-A0B5-E9B41717E62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C555208B-75F8-46DC-BB84-BB0DA3458377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="829" firstSheet="11" activeTab="18" xr2:uid="{35520F66-FEA5-4575-927A-C3FC8E8C1344}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="829" firstSheet="15" activeTab="19" xr2:uid="{35520F66-FEA5-4575-927A-C3FC8E8C1344}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Deck" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,10 @@
     <sheet name="Cann Edition" sheetId="17" r:id="rId17"/>
     <sheet name="Valentino Edition" sheetId="18" r:id="rId18"/>
     <sheet name="Existential Crisis Edition" sheetId="19" r:id="rId19"/>
+    <sheet name="Love Maps" sheetId="20" r:id="rId20"/>
+    <sheet name="Open Ended Questions" sheetId="21" r:id="rId21"/>
+    <sheet name="Rituals of Connection" sheetId="22" r:id="rId22"/>
+    <sheet name="Opportunity" sheetId="23" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1708" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2228" uniqueCount="1078">
   <si>
     <t>Card</t>
   </si>
@@ -2606,6 +2610,779 @@
 Use thought-provoking cards to find new dimensions in existing friendships as
 well as forge new ones. Invite over some friends, put the Cann on ice, and play
 the game that makes you *feel things*.</t>
+  </si>
+  <si>
+    <t>Name your partner's two closest friends.</t>
+  </si>
+  <si>
+    <t>What was your partner wearing when you first met?</t>
+  </si>
+  <si>
+    <t>What are your partner's hobbies?</t>
+  </si>
+  <si>
+    <t>Where was your partner born?</t>
+  </si>
+  <si>
+    <t>What stresses are facing your partner in the immediate future?</t>
+  </si>
+  <si>
+    <t>Describe in detail your partner's day, either today or yesterday.</t>
+  </si>
+  <si>
+    <t>When is your partner's birthday?</t>
+  </si>
+  <si>
+    <t>What is the date of your anniversary?</t>
+  </si>
+  <si>
+    <t>Who is your partner's favourite relative?</t>
+  </si>
+  <si>
+    <t>What is your partner's fondest dream, as yet unachieved?</t>
+  </si>
+  <si>
+    <t>What is your partner's favourite flower?</t>
+  </si>
+  <si>
+    <t>What is one of your partner's worst fears?</t>
+  </si>
+  <si>
+    <t>What is your partner's favourite time for making love?</t>
+  </si>
+  <si>
+    <t>What makes your partner feel most competent?</t>
+  </si>
+  <si>
+    <t>What turns your partner on sexually?</t>
+  </si>
+  <si>
+    <t>What is your partner's favourite food?</t>
+  </si>
+  <si>
+    <t>What is your partner's favourite way to spend an evening?</t>
+  </si>
+  <si>
+    <t>What personal improvements does your partner want to make in his or her life?</t>
+  </si>
+  <si>
+    <t>What kind of present would your partner like best?</t>
+  </si>
+  <si>
+    <t>What was one of your partner's best childhood experiences?</t>
+  </si>
+  <si>
+    <t>What was your partner's favourite vacation?</t>
+  </si>
+  <si>
+    <t>What is one of your partner's favourite ways of being soothed?</t>
+  </si>
+  <si>
+    <t>Who is your partner's greatest source of support (other than you)?</t>
+  </si>
+  <si>
+    <t>What is your partner's favourite sport?</t>
+  </si>
+  <si>
+    <t>What does your partner like to do with time off?</t>
+  </si>
+  <si>
+    <t>What is one of your partner's favourite weekend activities?</t>
+  </si>
+  <si>
+    <t>What is your partner's favourite getaway place?</t>
+  </si>
+  <si>
+    <t>What is your partner's favourite movie?</t>
+  </si>
+  <si>
+    <t>What are some of the important event coming up in your partner's life and how does he or she feel about them?</t>
+  </si>
+  <si>
+    <t>What are some of your partner's favourite ways to work out?</t>
+  </si>
+  <si>
+    <t>What is your partner's favourite cologne or perfume?</t>
+  </si>
+  <si>
+    <t>Who was your partner's best friend in childhood?</t>
+  </si>
+  <si>
+    <t>What is one of your partner's favourite magazines?</t>
+  </si>
+  <si>
+    <t>Name one of your partner's major rivals or "enemies".</t>
+  </si>
+  <si>
+    <t>What would be an ideal job for your partner?</t>
+  </si>
+  <si>
+    <t>What is your partner's greatest fear?</t>
+  </si>
+  <si>
+    <t>Who is your partner's least favourite relative?</t>
+  </si>
+  <si>
+    <t>What is your partner's favourite holiday?</t>
+  </si>
+  <si>
+    <t>What is your partner's favourite kind of reading?</t>
+  </si>
+  <si>
+    <t>What is your partner currently most sad about?</t>
+  </si>
+  <si>
+    <t>What is one of your partner's concern or worries?</t>
+  </si>
+  <si>
+    <t>What medical problems does your partner worry about?</t>
+  </si>
+  <si>
+    <t>What is your partner's worst childhood experience?</t>
+  </si>
+  <si>
+    <t>Which people does your partner most admire in the world? Name two.</t>
+  </si>
+  <si>
+    <t>Who is your partner's least favourite person you both know?</t>
+  </si>
+  <si>
+    <t>What is one of your partner's favourite desserts?</t>
+  </si>
+  <si>
+    <t>What is one of your partner's favourite novels?</t>
+  </si>
+  <si>
+    <t>What is your partner's favourite romantic restaurant?</t>
+  </si>
+  <si>
+    <t>What are two of your partner's aspirations, hopes, or wishes?</t>
+  </si>
+  <si>
+    <t>Does your partner have a secret ambition? What is it?</t>
+  </si>
+  <si>
+    <t>What food does your partner hate?</t>
+  </si>
+  <si>
+    <t>What is your partner's favourite animal?</t>
+  </si>
+  <si>
+    <t>What is your partner's favourite song?</t>
+  </si>
+  <si>
+    <t>What is your partner's favourite tree?</t>
+  </si>
+  <si>
+    <t>What is your partner's favourite colour?</t>
+  </si>
+  <si>
+    <t>What is your partner's favourite TV show?</t>
+  </si>
+  <si>
+    <t>Who is your partner's favourite poet?</t>
+  </si>
+  <si>
+    <t>What is your partner's favourite side of the bed?</t>
+  </si>
+  <si>
+    <t>What was your partner's most embarrassing moment?</t>
+  </si>
+  <si>
+    <t>Want to improve your relationship? These are questions you can ask your partner,
+as well as suggestions for things to do and say. Start with one or two and see how
+it goes, then come back for more.</t>
+  </si>
+  <si>
+    <t>How do you see your work changing in the future?</t>
+  </si>
+  <si>
+    <t>How do you feel about our physical home? Any architectural changes you'd like to make?</t>
+  </si>
+  <si>
+    <t>How would you compare yourself as a mother/father to your own mother/father?</t>
+  </si>
+  <si>
+    <t>What kind of person do you think our child(ren) wil become? Any fears? Any hopes?</t>
+  </si>
+  <si>
+    <t>Is our child like anyone in your family? Who?</t>
+  </si>
+  <si>
+    <t>How do you feel about your family right now? Have these feelings changed lately?</t>
+  </si>
+  <si>
+    <t>How do you feel about work right now?</t>
+  </si>
+  <si>
+    <t>How are you feelign now about being a mother/father?</t>
+  </si>
+  <si>
+    <t>What do you find exciting in life right now?</t>
+  </si>
+  <si>
+    <t>What are your biggest worries about the future?</t>
+  </si>
+  <si>
+    <t>How do you think we could have more fun in our life?</t>
+  </si>
+  <si>
+    <t>Who are your best allies and close friends right now? How have they changed or you changed?</t>
+  </si>
+  <si>
+    <t>How have your friendships changed lately? Have you grown closer to some friends? More distant from others?</t>
+  </si>
+  <si>
+    <t>Who in your life is most stressful for you? Why?</t>
+  </si>
+  <si>
+    <t>What do you need right now in a friend?</t>
+  </si>
+  <si>
+    <t>What things are missing in your life?</t>
+  </si>
+  <si>
+    <t>How have you changed in the last year?</t>
+  </si>
+  <si>
+    <t>Have your goals in life changed recently?</t>
+  </si>
+  <si>
+    <t>What are some of your life dreams right now?</t>
+  </si>
+  <si>
+    <t>What goes do you have for our family?</t>
+  </si>
+  <si>
+    <t>What goes do you have just for yourself right now?</t>
+  </si>
+  <si>
+    <t>What is one way you would like to change?</t>
+  </si>
+  <si>
+    <t>What legacy do you want our family to take from your family? From your culture?</t>
+  </si>
+  <si>
+    <t>What are some unfulfilled things in your life?</t>
+  </si>
+  <si>
+    <t>What would you change about our finances right now?</t>
+  </si>
+  <si>
+    <t>Where would you like to travel?</t>
+  </si>
+  <si>
+    <t>What adventures would you like to have before you die?</t>
+  </si>
+  <si>
+    <t>How has your outlook on life ch anged in the past two years?</t>
+  </si>
+  <si>
+    <t>If you could live one other person's life, whose life would you choose and why?</t>
+  </si>
+  <si>
+    <t>If you could live during any other time period in history, when would you choose to live and why?</t>
+  </si>
+  <si>
+    <t>What do you imagine your life would be like if you lived 100 years from now?</t>
+  </si>
+  <si>
+    <t>If you could design the perfect house for us, what would it look like?</t>
+  </si>
+  <si>
+    <t>If you could choose any other career or vocation other than what you do now, what would you choose and why?</t>
+  </si>
+  <si>
+    <t>What were the highlights and low-lights of your adolescence?</t>
+  </si>
+  <si>
+    <t>If you could wake up tomorrow with three new skills in which you excelled, what would they be and why?</t>
+  </si>
+  <si>
+    <t>If you could re-do any decade of your life, which decade would you choose and why?</t>
+  </si>
+  <si>
+    <t>What kind of year has this been for you? Tell me the story of your proudest moment.</t>
+  </si>
+  <si>
+    <t>How have you changed as a daughter or son?</t>
+  </si>
+  <si>
+    <t>How have you changed as a brother or sister?</t>
+  </si>
+  <si>
+    <t>What relatives have you felt closest to and why?</t>
+  </si>
+  <si>
+    <t>Who has been the most difficult person in your life (other than a partner or spouse) and why?</t>
+  </si>
+  <si>
+    <t>If you could change into any animal for 24 hours, what would it be and why?</t>
+  </si>
+  <si>
+    <t>Who was your childhood hero or heroine and why?</t>
+  </si>
+  <si>
+    <t>If you could live in any other country but your home country, which would you pick and why?</t>
+  </si>
+  <si>
+    <t>If you could experience being any other person for 24 hours, who would you pick and why?</t>
+  </si>
+  <si>
+    <t>If you could be a genius in any art, music, drama, or dance, which talent would you choose and why?</t>
+  </si>
+  <si>
+    <t>If you could be a superstar in any sport, which sport would you choose and why?</t>
+  </si>
+  <si>
+    <t>If you could be the richest person in the world, what would you do with your money?</t>
+  </si>
+  <si>
+    <t>If you could look like anyone else in the world, who would you pick and why?</t>
+  </si>
+  <si>
+    <t>If you could change one characteristic about yourself, what would it be and why?</t>
+  </si>
+  <si>
+    <t>Communicating appreciation for your partner</t>
+  </si>
+  <si>
+    <t>Bringing friends into our home</t>
+  </si>
+  <si>
+    <t>Meal times</t>
+  </si>
+  <si>
+    <t>Celebrating success</t>
+  </si>
+  <si>
+    <t>Communicating daily appreciations</t>
+  </si>
+  <si>
+    <t>Throwing small dinner parties</t>
+  </si>
+  <si>
+    <t>Initiating lovemaking</t>
+  </si>
+  <si>
+    <t>Refusing lovemaking</t>
+  </si>
+  <si>
+    <t>Talking about how to improve lovemaking</t>
+  </si>
+  <si>
+    <t>Celebrating birthdays</t>
+  </si>
+  <si>
+    <t>Celebrating anniversaries</t>
+  </si>
+  <si>
+    <t>Celebrating holidays</t>
+  </si>
+  <si>
+    <t>Renewing ourselves when we are fatigued or burned out</t>
+  </si>
+  <si>
+    <t>Dealing with bad luck or hard days</t>
+  </si>
+  <si>
+    <t>Getting ready for bed</t>
+  </si>
+  <si>
+    <t>Falling asleep</t>
+  </si>
+  <si>
+    <t>Waking in the morning</t>
+  </si>
+  <si>
+    <t>Bringing up issues in our relationship</t>
+  </si>
+  <si>
+    <t>Expressing needs</t>
+  </si>
+  <si>
+    <t>Taking leave of one another (saying goodbye)</t>
+  </si>
+  <si>
+    <t>Reunions (saying hello)</t>
+  </si>
+  <si>
+    <t>Discussing stressful events</t>
+  </si>
+  <si>
+    <t>Spending time together on weekends</t>
+  </si>
+  <si>
+    <t>Planning and going on dates</t>
+  </si>
+  <si>
+    <t>Taking care of one another when one of us gets sick</t>
+  </si>
+  <si>
+    <t>Spending time with in-laws/extended family</t>
+  </si>
+  <si>
+    <t>Spending time with the kids in the evenings</t>
+  </si>
+  <si>
+    <t>Getting the kids ready for school in the morning</t>
+  </si>
+  <si>
+    <t>Shopping for groceries</t>
+  </si>
+  <si>
+    <t>Planning small adventures near our hometown (staycations)</t>
+  </si>
+  <si>
+    <t>Dreaming of the future</t>
+  </si>
+  <si>
+    <t>Setting goals together</t>
+  </si>
+  <si>
+    <t>Making meals at home and preparing recipes together</t>
+  </si>
+  <si>
+    <t>Planning for the upcoming week</t>
+  </si>
+  <si>
+    <t>Sharing tea or coffee together</t>
+  </si>
+  <si>
+    <t>Learning or taking classes together (dancing, cooking, etc.)</t>
+  </si>
+  <si>
+    <t>Participating in individual or joint hobbies</t>
+  </si>
+  <si>
+    <t>Spending time in nature</t>
+  </si>
+  <si>
+    <t>Running errands</t>
+  </si>
+  <si>
+    <t>Volunteering in the community</t>
+  </si>
+  <si>
+    <t>Playing board games at home</t>
+  </si>
+  <si>
+    <t>Exercising together</t>
+  </si>
+  <si>
+    <t>Sharing highs and lows</t>
+  </si>
+  <si>
+    <t>Staying in touch throughout the day using technology (texting/other message rituals)</t>
+  </si>
+  <si>
+    <t>Telling each other when we are overwhelmed or flooded</t>
+  </si>
+  <si>
+    <t>Making breakfast</t>
+  </si>
+  <si>
+    <t>Lazy weekend mornings at home</t>
+  </si>
+  <si>
+    <t>Being playful and silly with one another</t>
+  </si>
+  <si>
+    <t>Staying connected while we are apart (during the work day, when one of us is traveling, etc.)</t>
+  </si>
+  <si>
+    <t>Using time while travelling together (drive time, flying time, etc.)</t>
+  </si>
+  <si>
+    <t>Giving back to our community together</t>
+  </si>
+  <si>
+    <t>Fostering a sense of adventure in our lives</t>
+  </si>
+  <si>
+    <t>Planning and going on vacations</t>
+  </si>
+  <si>
+    <t>What is your partner's favourite musical group, composer, or instrument?</t>
+  </si>
+  <si>
+    <t>Having a big party at home</t>
+  </si>
+  <si>
+    <t>Disconnecting from devices and technology for a period of time in order to give undivided attention to each other</t>
+  </si>
+  <si>
+    <t>Open-ended questions cannot be answered with a simple 'yes' or 'no'. They have
+stories for answers. Uncover your hopes and dreams to deepen your understanding.
+Take turns asking each other questions. If your partner doesn't want to answer the
+question, pick another card. Do not be judgemental or critical as you listen to your
+partner's answer. Instead, be a 'dream detective'. Alternate roles as speaker and
+listener.</t>
+  </si>
+  <si>
+    <t>It's the little things that build trust, friendship, and closeness. This deck will help
+you recognize and act on the small, everyday moments that build intimacy in
+meaningful ways.
+It's important to have fun together as a couple! When you are at a loss for ideas,
+use these activity suggestions to plan your next date night or outing. Swipe
+through until you find something you both want to do.</t>
+  </si>
+  <si>
+    <t>Bring home something special for your partner (like flowers).</t>
+  </si>
+  <si>
+    <t>Get tickets to an exciting concert.</t>
+  </si>
+  <si>
+    <t>Take a class together.</t>
+  </si>
+  <si>
+    <t>Learn a new language and culture together. Visit that country if possible.</t>
+  </si>
+  <si>
+    <t>Find our your partner's favourite play and go see it.</t>
+  </si>
+  <si>
+    <t>Give your partner a full day off from household chores.</t>
+  </si>
+  <si>
+    <t>Making a sexy music playlist just for your partner.</t>
+  </si>
+  <si>
+    <t>Plan a picnic for the two of you.</t>
+  </si>
+  <si>
+    <t>Return to your honeymoon place or revisit a favourite location.</t>
+  </si>
+  <si>
+    <t>Ritual of Connection is a method of turning towards your partner that can be
+counted on. Use this deck to decide which rituals to include in your lives together.
+Select a card and discuss whether you would like to incorporate this ritual in your
+relationship, and if so, exactly how it should go, who should do what and when,
+and how it should end. Be sure to talk about if and why this is important to you,
+and how this ritual was handled (or mishandled) in your family or in previous
+relationships.</t>
+  </si>
+  <si>
+    <t>Buy a surprise present for your partner.</t>
+  </si>
+  <si>
+    <t>Plan a reunion party of all your partner's friends.</t>
+  </si>
+  <si>
+    <t>Discover your partner's turn ons and incorporate them into lovemaking.</t>
+  </si>
+  <si>
+    <t>Find out your partner's favourite movies and watch them together.</t>
+  </si>
+  <si>
+    <t>Take a leisurely bath together.</t>
+  </si>
+  <si>
+    <t>Go out to dinner and ask your partner questions about how their life is going.</t>
+  </si>
+  <si>
+    <t>Go to a wine tasting party.</t>
+  </si>
+  <si>
+    <t>Plan a candlelight dinner.</t>
+  </si>
+  <si>
+    <t>Find out your partner's favourite hero(ine) and read a book about him(her).</t>
+  </si>
+  <si>
+    <t>Go out dancing.</t>
+  </si>
+  <si>
+    <t>Plan a weekend camping trip together.</t>
+  </si>
+  <si>
+    <t>Look through an online store your partner likes and order something from it to surprise them.</t>
+  </si>
+  <si>
+    <t>Go clothes shopping for your partner and buy something you would like to see them in.</t>
+  </si>
+  <si>
+    <t>Bring home your partner's favourite dessert (like chocolates), prepare their favourite tea or coffee, and serve them.</t>
+  </si>
+  <si>
+    <t>Write a love letter and mail it to your partner.</t>
+  </si>
+  <si>
+    <t>Prepare a surprise breakfast in bed.</t>
+  </si>
+  <si>
+    <t>Plan some way that you would like to improve your home.</t>
+  </si>
+  <si>
+    <t>Plan a surprise party for your partner.</t>
+  </si>
+  <si>
+    <t>Surprise your partner with two tickets to some interesting place or event.</t>
+  </si>
+  <si>
+    <t>Buy tickets to a play that your partner wants to see.</t>
+  </si>
+  <si>
+    <t>Find or write a poem that expresses a genuine appreciation of your partner.</t>
+  </si>
+  <si>
+    <t>Plan a weekend getaway.</t>
+  </si>
+  <si>
+    <t>Plan a Valentine's getaway.</t>
+  </si>
+  <si>
+    <t>Plan a date.</t>
+  </si>
+  <si>
+    <t>Plan a cruise or vacation.</t>
+  </si>
+  <si>
+    <t>Find out your partner's favourite novel and read it.</t>
+  </si>
+  <si>
+    <t>Plan a monthly book club for the two of you and switch turns choosing the book.</t>
+  </si>
+  <si>
+    <t>Spend time together in garden.</t>
+  </si>
+  <si>
+    <t>Check our nearby museums together. (Often museums have discounted or free days!)</t>
+  </si>
+  <si>
+    <t>Read the local events paper and go to a festival or cultural event in your city.</t>
+  </si>
+  <si>
+    <t>Spend the day doing an activity or hobby of your partner's choosing.</t>
+  </si>
+  <si>
+    <t>Plan to attend a volunteering event.</t>
+  </si>
+  <si>
+    <t>Plan a scavenger hunt for your partner around your home or around the city.</t>
+  </si>
+  <si>
+    <t>Rent bikes and explore the city together.</t>
+  </si>
+  <si>
+    <t>Cook a new recipe together that you've been wanting to try.</t>
+  </si>
+  <si>
+    <t>Wake up early and watch the sunrise together.</t>
+  </si>
+  <si>
+    <t>Go to a comedy show.</t>
+  </si>
+  <si>
+    <t>Learn how to paint or do pottery together.</t>
+  </si>
+  <si>
+    <t>Go to an amusement park.</t>
+  </si>
+  <si>
+    <t>Have a water balloon or super-soaker fight on a hot summer day.</t>
+  </si>
+  <si>
+    <t>Build a snowman together and  have a snowball fight.</t>
+  </si>
+  <si>
+    <t>Do an exercise challenge together.</t>
+  </si>
+  <si>
+    <t>Disconnect to connect: decide on a period of time together that electronic devices will not be turned on at home.</t>
+  </si>
+  <si>
+    <t>Watch a TED talk or other inspiring video together to learn a new concept together.</t>
+  </si>
+  <si>
+    <t>View your old home videos of special couple or family memories.</t>
+  </si>
+  <si>
+    <t>Develop a dinner menu together that includes both your partner's and your favourite dishes.</t>
+  </si>
+  <si>
+    <t>Plan a game night. Enjoy a night in playing board/card games together.</t>
+  </si>
+  <si>
+    <t>Give your partner a special massage. (If you don't know how, watch a YouTube video or get a book and learn.)</t>
+  </si>
+  <si>
+    <t>Leave little notes all over the house with small endearments and express genuine appreciation.</t>
+  </si>
+  <si>
+    <t>Make up words for a secret language together.</t>
+  </si>
+  <si>
+    <t>Spend a rainy day cuddled on the couch with a good movie or TV show and order food in.</t>
+  </si>
+  <si>
+    <t>Binge watch your favourite TV show.</t>
+  </si>
+  <si>
+    <t>Cook dinner at home.</t>
+  </si>
+  <si>
+    <t>Have dessert in bed.</t>
+  </si>
+  <si>
+    <t>Take a romantic bath.</t>
+  </si>
+  <si>
+    <t>Try a new hobby together.</t>
+  </si>
+  <si>
+    <t>Video call one another.</t>
+  </si>
+  <si>
+    <t>Take a walk around your neighbourhood.</t>
+  </si>
+  <si>
+    <t>Read together.</t>
+  </si>
+  <si>
+    <t>Do YouTube dance lessons.</t>
+  </si>
+  <si>
+    <t>Have a backyard picnic.</t>
+  </si>
+  <si>
+    <t>Go through old photos.</t>
+  </si>
+  <si>
+    <t>Garden together.</t>
+  </si>
+  <si>
+    <t>Watch each other's favourite movies.</t>
+  </si>
+  <si>
+    <t>Attend a virtual bartending/mixology class.</t>
+  </si>
+  <si>
+    <t>Do the other person's favourite thing (and trade off)</t>
+  </si>
+  <si>
+    <t>Listen to music together.</t>
+  </si>
+  <si>
+    <t>Meditate and/or do yoga.</t>
+  </si>
+  <si>
+    <t>Play video games.</t>
+  </si>
+  <si>
+    <t>Watch the sunset.</t>
+  </si>
+  <si>
+    <t>Gotmann</t>
+  </si>
+  <si>
+    <t>An important factor in relationship success is knowing about your partner's inner
+world; we call this idea Love Maps.
+Swipe through the deck and see if you can answer the question as it relates to
+your partner. Then switch roles. Have your partner swipe through the deck and
+try to answer as it pertains to your world. Don't keep score. The goal is
+meaningful conversation and connection.</t>
   </si>
 </sst>
 </file>
@@ -2647,10 +3424,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7538,7 +8318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{711D2D5C-5401-4F25-8002-549E2C45E37A}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -8396,6 +9176,2156 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1659DC61-407C-426F-AA60-143EAC012977}">
+  <dimension ref="A1:B65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" t="s">
+        <v>886</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D0304A-DF57-4437-A329-33A2BEA0B3B1}">
+  <dimension ref="A1:B55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" t="s">
+        <v>937</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266716F5-2382-4BA3-89BC-34C748FDC5CA}">
+  <dimension ref="A1:B60"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" t="s">
+        <v>989</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EB6A34-6766-4F36-ABD4-63EFDDDDD80E}">
+  <dimension ref="A1:B84"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1B56EE-3E41-4700-94E1-99053861750B}">
   <dimension ref="A1:B56"/>

</xml_diff>

<commit_message>
interface changes: add instructinos, change deck hover information, change load screen instruction width
</commit_message>
<xml_diff>
--- a/data/WNRS.xlsx
+++ b/data/WNRS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KayJan\test-app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C555208B-75F8-46DC-BB84-BB0DA3458377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20DA916-7C38-443B-B355-C0F48E0D7CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="829" firstSheet="15" activeTab="19" xr2:uid="{35520F66-FEA5-4575-927A-C3FC8E8C1344}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="829" firstSheet="5" activeTab="7" xr2:uid="{35520F66-FEA5-4575-927A-C3FC8E8C1344}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Deck" sheetId="1" r:id="rId1"/>
@@ -2584,10 +2584,6 @@
     <t>There's always another layer to anyone you (think you) know</t>
   </si>
   <si>
-    <t>The intention behind this set of questions and wildcards is to dig deeper with
-the people in our lives that we think we know best.</t>
-  </si>
-  <si>
     <t>Despite being physically apart, our emotional connections don't need to suffer.</t>
   </si>
   <si>
@@ -3383,6 +3379,11 @@
 your partner. Then switch roles. Have your partner swipe through the deck and
 try to answer as it pertains to your world. Don't keep score. The goal is
 meaningful conversation and connection.</t>
+  </si>
+  <si>
+    <t>Does knowing someone for long equate to knowing them deeply? The intention
+behind this set of questions and wildcards is to dig deeper with the people in
+our lives that we think we know best.</t>
   </si>
 </sst>
 </file>
@@ -4652,7 +4653,7 @@
         <v>2</v>
       </c>
       <c r="C84" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
@@ -4707,7 +4708,7 @@
         <v>2</v>
       </c>
       <c r="C89" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
@@ -4762,7 +4763,7 @@
         <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
@@ -4828,7 +4829,7 @@
         <v>3</v>
       </c>
       <c r="C100" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -4850,7 +4851,7 @@
         <v>3</v>
       </c>
       <c r="C102" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
@@ -6461,7 +6462,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -7767,7 +7768,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -9180,7 +9181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1659DC61-407C-426F-AA60-143EAC012977}">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -9189,7 +9190,7 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -9197,7 +9198,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -9205,7 +9206,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -9224,7 +9225,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9232,7 +9233,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -9240,7 +9241,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -9248,7 +9249,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -9256,7 +9257,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -9264,7 +9265,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -9272,7 +9273,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -9280,7 +9281,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -9288,7 +9289,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -9296,7 +9297,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -9304,7 +9305,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -9312,7 +9313,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -9320,7 +9321,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -9328,7 +9329,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -9336,7 +9337,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -9344,7 +9345,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -9352,7 +9353,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -9360,7 +9361,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -9368,7 +9369,7 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -9376,7 +9377,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -9384,7 +9385,7 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -9392,7 +9393,7 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -9400,7 +9401,7 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -9408,7 +9409,7 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -9416,7 +9417,7 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -9424,7 +9425,7 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -9432,7 +9433,7 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -9440,7 +9441,7 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -9448,7 +9449,7 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -9456,7 +9457,7 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -9464,7 +9465,7 @@
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -9472,7 +9473,7 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -9480,7 +9481,7 @@
         <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -9488,7 +9489,7 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -9496,7 +9497,7 @@
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -9504,7 +9505,7 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -9512,7 +9513,7 @@
         <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -9520,7 +9521,7 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -9528,7 +9529,7 @@
         <v>2</v>
       </c>
       <c r="B44" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -9536,7 +9537,7 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -9544,7 +9545,7 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -9552,7 +9553,7 @@
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -9560,7 +9561,7 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -9568,7 +9569,7 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -9576,7 +9577,7 @@
         <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -9584,7 +9585,7 @@
         <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -9592,7 +9593,7 @@
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -9600,7 +9601,7 @@
         <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -9608,7 +9609,7 @@
         <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -9616,7 +9617,7 @@
         <v>2</v>
       </c>
       <c r="B55" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -9624,7 +9625,7 @@
         <v>2</v>
       </c>
       <c r="B56" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -9632,7 +9633,7 @@
         <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -9640,7 +9641,7 @@
         <v>2</v>
       </c>
       <c r="B58" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -9648,7 +9649,7 @@
         <v>2</v>
       </c>
       <c r="B59" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -9656,7 +9657,7 @@
         <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -9664,7 +9665,7 @@
         <v>2</v>
       </c>
       <c r="B61" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -9672,7 +9673,7 @@
         <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -9680,7 +9681,7 @@
         <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -9688,7 +9689,7 @@
         <v>2</v>
       </c>
       <c r="B64" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -9696,7 +9697,7 @@
         <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
   </sheetData>
@@ -9719,7 +9720,7 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -9727,7 +9728,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -9735,7 +9736,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -9754,7 +9755,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -9762,7 +9763,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -9770,7 +9771,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -9778,7 +9779,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -9786,7 +9787,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -9794,7 +9795,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -9802,7 +9803,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -9810,7 +9811,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -9818,7 +9819,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -9826,7 +9827,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -9834,7 +9835,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -9842,7 +9843,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -9850,7 +9851,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -9858,7 +9859,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -9866,7 +9867,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -9874,7 +9875,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -9882,7 +9883,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -9890,7 +9891,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -9898,7 +9899,7 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -9906,7 +9907,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -9914,7 +9915,7 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -9922,7 +9923,7 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -9930,7 +9931,7 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -9938,7 +9939,7 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -9946,7 +9947,7 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -9954,7 +9955,7 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -9962,7 +9963,7 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -9970,7 +9971,7 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -9978,7 +9979,7 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -9986,7 +9987,7 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -9994,7 +9995,7 @@
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -10002,7 +10003,7 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -10010,7 +10011,7 @@
         <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -10018,7 +10019,7 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -10026,7 +10027,7 @@
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -10034,7 +10035,7 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -10042,7 +10043,7 @@
         <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -10050,7 +10051,7 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -10058,7 +10059,7 @@
         <v>2</v>
       </c>
       <c r="B44" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -10066,7 +10067,7 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -10074,7 +10075,7 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -10082,7 +10083,7 @@
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -10090,7 +10091,7 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -10098,7 +10099,7 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -10106,7 +10107,7 @@
         <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -10114,7 +10115,7 @@
         <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -10122,7 +10123,7 @@
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -10130,7 +10131,7 @@
         <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -10138,7 +10139,7 @@
         <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -10146,7 +10147,7 @@
         <v>2</v>
       </c>
       <c r="B55" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
   </sheetData>
@@ -10169,7 +10170,7 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -10177,7 +10178,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -10185,7 +10186,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -10204,7 +10205,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -10212,7 +10213,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -10220,7 +10221,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -10228,7 +10229,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -10236,7 +10237,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -10244,7 +10245,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -10252,7 +10253,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -10260,7 +10261,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -10268,7 +10269,7 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -10276,7 +10277,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -10284,7 +10285,7 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -10292,7 +10293,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -10300,7 +10301,7 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -10308,7 +10309,7 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -10316,7 +10317,7 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -10324,7 +10325,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -10332,7 +10333,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -10340,7 +10341,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -10348,7 +10349,7 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -10356,7 +10357,7 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -10364,7 +10365,7 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -10372,7 +10373,7 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -10380,7 +10381,7 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -10388,7 +10389,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -10396,7 +10397,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -10404,7 +10405,7 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -10412,7 +10413,7 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -10420,7 +10421,7 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -10428,7 +10429,7 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -10436,7 +10437,7 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -10444,7 +10445,7 @@
         <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -10452,7 +10453,7 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -10460,7 +10461,7 @@
         <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -10468,7 +10469,7 @@
         <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -10476,7 +10477,7 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -10484,7 +10485,7 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -10492,7 +10493,7 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -10500,7 +10501,7 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -10508,7 +10509,7 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -10516,7 +10517,7 @@
         <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -10524,7 +10525,7 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -10532,7 +10533,7 @@
         <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -10540,7 +10541,7 @@
         <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -10548,7 +10549,7 @@
         <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -10556,7 +10557,7 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -10564,7 +10565,7 @@
         <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -10572,7 +10573,7 @@
         <v>3</v>
       </c>
       <c r="B52" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -10580,7 +10581,7 @@
         <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -10588,7 +10589,7 @@
         <v>3</v>
       </c>
       <c r="B54" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -10596,7 +10597,7 @@
         <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -10604,7 +10605,7 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -10612,7 +10613,7 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -10620,7 +10621,7 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -10628,7 +10629,7 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -10636,7 +10637,7 @@
         <v>3</v>
       </c>
       <c r="B60" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
   </sheetData>
@@ -10659,7 +10660,7 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -10667,7 +10668,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -10675,7 +10676,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -10694,7 +10695,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -10702,7 +10703,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -10710,7 +10711,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -10718,7 +10719,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -10726,7 +10727,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -10734,7 +10735,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -10742,7 +10743,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -10750,7 +10751,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -10758,7 +10759,7 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -10766,7 +10767,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -10774,7 +10775,7 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -10782,7 +10783,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -10790,7 +10791,7 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -10798,7 +10799,7 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -10806,7 +10807,7 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -10814,7 +10815,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -10822,7 +10823,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -10830,7 +10831,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -10838,7 +10839,7 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -10846,7 +10847,7 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -10854,7 +10855,7 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -10862,7 +10863,7 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -10870,7 +10871,7 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -10878,7 +10879,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -10886,7 +10887,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -10894,7 +10895,7 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -10902,7 +10903,7 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -10910,7 +10911,7 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -10918,7 +10919,7 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -10926,7 +10927,7 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -10934,7 +10935,7 @@
         <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -10942,7 +10943,7 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -10950,7 +10951,7 @@
         <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -10958,7 +10959,7 @@
         <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -10966,7 +10967,7 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -10974,7 +10975,7 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -10982,7 +10983,7 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -10990,7 +10991,7 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -10998,7 +10999,7 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -11006,7 +11007,7 @@
         <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -11014,7 +11015,7 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -11022,7 +11023,7 @@
         <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -11030,7 +11031,7 @@
         <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -11038,7 +11039,7 @@
         <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -11046,7 +11047,7 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -11054,7 +11055,7 @@
         <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -11062,7 +11063,7 @@
         <v>3</v>
       </c>
       <c r="B52" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -11070,7 +11071,7 @@
         <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -11078,7 +11079,7 @@
         <v>3</v>
       </c>
       <c r="B54" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -11086,7 +11087,7 @@
         <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -11094,7 +11095,7 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -11102,7 +11103,7 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -11110,7 +11111,7 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -11118,7 +11119,7 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -11126,7 +11127,7 @@
         <v>3</v>
       </c>
       <c r="B60" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -11134,7 +11135,7 @@
         <v>3</v>
       </c>
       <c r="B61" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -11142,7 +11143,7 @@
         <v>3</v>
       </c>
       <c r="B62" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -11150,7 +11151,7 @@
         <v>3</v>
       </c>
       <c r="B63" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -11158,7 +11159,7 @@
         <v>3</v>
       </c>
       <c r="B64" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -11166,7 +11167,7 @@
         <v>3</v>
       </c>
       <c r="B65" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -11174,7 +11175,7 @@
         <v>3</v>
       </c>
       <c r="B66" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -11182,7 +11183,7 @@
         <v>3</v>
       </c>
       <c r="B67" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -11190,7 +11191,7 @@
         <v>3</v>
       </c>
       <c r="B68" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -11198,7 +11199,7 @@
         <v>3</v>
       </c>
       <c r="B69" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -11206,7 +11207,7 @@
         <v>3</v>
       </c>
       <c r="B70" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -11214,7 +11215,7 @@
         <v>3</v>
       </c>
       <c r="B71" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -11222,7 +11223,7 @@
         <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -11230,7 +11231,7 @@
         <v>3</v>
       </c>
       <c r="B73" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -11238,7 +11239,7 @@
         <v>3</v>
       </c>
       <c r="B74" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -11246,7 +11247,7 @@
         <v>3</v>
       </c>
       <c r="B75" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -11254,7 +11255,7 @@
         <v>3</v>
       </c>
       <c r="B76" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -11262,7 +11263,7 @@
         <v>3</v>
       </c>
       <c r="B77" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -11270,7 +11271,7 @@
         <v>3</v>
       </c>
       <c r="B78" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -11278,7 +11279,7 @@
         <v>3</v>
       </c>
       <c r="B79" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -11286,7 +11287,7 @@
         <v>3</v>
       </c>
       <c r="B80" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
@@ -11294,7 +11295,7 @@
         <v>3</v>
       </c>
       <c r="B81" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -11302,7 +11303,7 @@
         <v>3</v>
       </c>
       <c r="B82" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -11310,7 +11311,7 @@
         <v>3</v>
       </c>
       <c r="B83" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -11318,7 +11319,7 @@
         <v>3</v>
       </c>
       <c r="B84" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
   </sheetData>
@@ -13915,7 +13916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B8EA38-56AE-433B-9F6B-066A2B5BF62F}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -13932,14 +13933,14 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>820</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>819</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v1.0.21 add new deck to WNRS
</commit_message>
<xml_diff>
--- a/data/WNRS.xlsx
+++ b/data/WNRS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KayJan/test-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D418E4-93AF-1745-8E81-250EE59D79AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F4FB6B-67EE-5F46-B663-37E92BC85FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-2140" windowWidth="38400" windowHeight="19400" tabRatio="829" activeTab="3" xr2:uid="{35520F66-FEA5-4575-927A-C3FC8E8C1344}"/>
+    <workbookView xWindow="-38400" yWindow="-5320" windowWidth="38400" windowHeight="21100" tabRatio="829" firstSheet="12" activeTab="23" xr2:uid="{35520F66-FEA5-4575-927A-C3FC8E8C1344}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Deck" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <sheet name="Open Ended Questions" sheetId="21" r:id="rId21"/>
     <sheet name="Rituals of Connection" sheetId="22" r:id="rId22"/>
     <sheet name="Opportunity" sheetId="23" r:id="rId23"/>
+    <sheet name="Couple" sheetId="24" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2308" uniqueCount="1098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2665" uniqueCount="1275">
   <si>
     <t>Card</t>
   </si>
@@ -3444,6 +3445,546 @@
   </si>
   <si>
     <t>What's your most vivid\n valentine's day memory?</t>
+  </si>
+  <si>
+    <t>Couple Questions</t>
+  </si>
+  <si>
+    <t>One of the most important things in a relationship is learning about your partner.
+You can know what to expect from them and can figure out if you two are a good
+match. It’s important to be non-judgmental when asking and answering these
+questions. It’s not about telling your partner the things they do wrong or the
+things you want from them. It’s about working together as a couple to build a
+healthy relationship.</t>
+  </si>
+  <si>
+    <t>What's your ideal way to spend a vacation?</t>
+  </si>
+  <si>
+    <t>What makes you dislike a person?</t>
+  </si>
+  <si>
+    <t>Do you think you are a confident person? Why or why not?</t>
+  </si>
+  <si>
+    <t>What about yourself are you most proud of?</t>
+  </si>
+  <si>
+    <t>What would the best version of you be like?</t>
+  </si>
+  <si>
+    <t>What life experiences did you miss out on?</t>
+  </si>
+  <si>
+    <t>When are you the most "you"?</t>
+  </si>
+  <si>
+    <t>How did you fall out with some of your previously close friends?</t>
+  </si>
+  <si>
+    <t>Are you happy with the people you surround yourself with? Why or why not?</t>
+  </si>
+  <si>
+    <t>What musical instrument do you wish you could play?</t>
+  </si>
+  <si>
+    <t>When has a mundane occurrence or chance completely changed the course of your life? What is the nicest compliment you've received?</t>
+  </si>
+  <si>
+    <t>What age would you like to live to?</t>
+  </si>
+  <si>
+    <t>If you could travel to any country in the world for one month, where would you go? What is your favorite memory of someone who isn't in your life anymore?</t>
+  </si>
+  <si>
+    <t>How superstitious are you?</t>
+  </si>
+  <si>
+    <t>What has been a recurring theme in your life?</t>
+  </si>
+  <si>
+    <t>What was your most inappropriate or embarrassing fart?</t>
+  </si>
+  <si>
+    <t>What do you think happens after death?</t>
+  </si>
+  <si>
+    <t>What are your top 5 rules for life?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What's your favorite thing in your / our house? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What book or movie do you wish you could experience for the first time again? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you had a friend who spoke to you the same way you speak to yourself, would you keep them as a friend? </t>
+  </si>
+  <si>
+    <t>What petty thing that people do really gets on your nerves? What brings meaning to your life?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is something you wish you could say to people but can’t? What are some of the most attractive traits a person can have? What's a secret you've never told anyone? </t>
+  </si>
+  <si>
+    <t>What small pleasures do you enjoy the most?</t>
+  </si>
+  <si>
+    <t>Who is the most irritating person you know?</t>
+  </si>
+  <si>
+    <t>What has been your biggest screw up so far?</t>
+  </si>
+  <si>
+    <t>What have you struggled with your entire life?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the most significant change you would like to make in your life? What do you want out of life? </t>
+  </si>
+  <si>
+    <t>What calms you down the most?</t>
+  </si>
+  <si>
+    <t>What are kinds of things do you find repulsive?</t>
+  </si>
+  <si>
+    <t>What would your perfect life look like?</t>
+  </si>
+  <si>
+    <t>If you received a salary to follow whatever passion you wanted to, what would you do?</t>
+  </si>
+  <si>
+    <t>What's your most embarrassing story about being sick?</t>
+  </si>
+  <si>
+    <t>What friend have you not thought about in a long time?</t>
+  </si>
+  <si>
+    <t>What's the craziest thing that has happened at a job you worked at?</t>
+  </si>
+  <si>
+    <t>Who do you act nice around but secretly dislike?</t>
+  </si>
+  <si>
+    <t>If money was no object, and with no input from me, how would you decorate your / our house? How good are you at reading people?</t>
+  </si>
+  <si>
+    <t>Are you hopeful about your future?</t>
+  </si>
+  <si>
+    <t>Who do you want to be more like or who do you look up to most?</t>
+  </si>
+  <si>
+    <t>What were the healthiest and unhealthiest periods of your life?</t>
+  </si>
+  <si>
+    <t>What's the worst emotional or mental anguish you've endured?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What do you like most about where we live? </t>
+  </si>
+  <si>
+    <t>What do you worry about?</t>
+  </si>
+  <si>
+    <t>What's something you screwed up and then tried to hide?</t>
+  </si>
+  <si>
+    <t>What's the scariest / creepiest place you have ever been?</t>
+  </si>
+  <si>
+    <t>Do you think the world is improving or getting worse? Why?</t>
+  </si>
+  <si>
+    <t>How do you think society is changing? Do you think we'll change with it?</t>
+  </si>
+  <si>
+    <t>What’s the worst thing that people are proud of?</t>
+  </si>
+  <si>
+    <t>What’s the biggest betrayal you have ever experienced?</t>
+  </si>
+  <si>
+    <t>What would be the greatest gift to receive?</t>
+  </si>
+  <si>
+    <t>What is something that you are dreading?</t>
+  </si>
+  <si>
+    <t>What makes you feel super fancy?</t>
+  </si>
+  <si>
+    <t>What would you want your obituary to say?</t>
+  </si>
+  <si>
+    <t>What has taken up too much of your life?</t>
+  </si>
+  <si>
+    <t>What’s the most disheartening and heartening realization you have come to?</t>
+  </si>
+  <si>
+    <t>What was the hardest lesson you’ve had to learn?</t>
+  </si>
+  <si>
+    <t>Would you take 3 million dollars if it meant that the person you hate most in the world gets 9 million? What part of you as a person still needs a lot of work?</t>
+  </si>
+  <si>
+    <t>What are some words of wisdom that have stuck with you all these years?</t>
+  </si>
+  <si>
+    <t>How well do you know yourself?</t>
+  </si>
+  <si>
+    <t>What is your best (not worst) flaw?</t>
+  </si>
+  <si>
+    <t>How forgiving are you?</t>
+  </si>
+  <si>
+    <t>Tell me about a time you almost died.</t>
+  </si>
+  <si>
+    <t>Are you ashamed of anything you did in the past? If you are comfortable talking about it, what was it? Do you prefer living in the countryside, in a town, or in a big city? Why?</t>
+  </si>
+  <si>
+    <t>What's your fondest memory of a tree?</t>
+  </si>
+  <si>
+    <t>What are some of the most pleasant sensations for you?</t>
+  </si>
+  <si>
+    <t>Are you happy with the career path you chose or do you wish you had chosen a different career? What's the most unethical thing you do regularly?</t>
+  </si>
+  <si>
+    <t>What is way more difficult than it sounds?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What job do you think you were born to do? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What's the biggest financial mistake you've made? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What makes you lose faith in humanity when you think about it? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What was the most painful thing to hear? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What biases do you think you have? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are you battling that you don’t tell anyone about? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What luxury do you enjoy treating yourself to? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What do you most like to do when you have alone time? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is normal now that will be considered unethical and barbaric in 100 years? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you're gone when you want to be remembered for? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If there was a horrible accident and you were unconscious and on life support, how long would you want to be on life support? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you believe in good luck and bad luck? How about things that are lucky or unlucky? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you had a million dollars to give to any charity, what type of charity would you give it to? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What's something that a lot of people are afraid of, but you aren't? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you could open a business what type of business would you open? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What can someone do that makes them immediately unattractive to you, no matter how attractive they are physically? </t>
+  </si>
+  <si>
+    <t>What untrue thing did you believe for an incredibly long time?</t>
+  </si>
+  <si>
+    <t>What were the three most important turning points in your life?</t>
+  </si>
+  <si>
+    <t>What animal are you most afraid of?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What scandal happened in your neighbor or town when you were growing up? How well do you think you would handle prison? </t>
+  </si>
+  <si>
+    <t>What's the most awkward social situation you've been in?</t>
+  </si>
+  <si>
+    <t>What is something that scares you on a daily basis?</t>
+  </si>
+  <si>
+    <t>When was the last time you cried?</t>
+  </si>
+  <si>
+    <t>What's the most peaceful/restful night of sleep you've had?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What's the most dangerous, thrill-seeking thing you would consider doing? What's your biggest regret? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is it better to trust people or not trust people? And why? </t>
+  </si>
+  <si>
+    <t>What do you think your best and worst personality traits are? Who do you miss the most?</t>
+  </si>
+  <si>
+    <t>What is the hardest life lesson you've had to learn?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What do you take for granted? </t>
+  </si>
+  <si>
+    <t>What's the most stressful situation you've been in? How did you handle it? What's the most ambitious thing you've attempted?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How often do you change your opinions or how you view the world? What's the biggest opportunity you were given? </t>
+  </si>
+  <si>
+    <t>What is something we should enjoy more because it won't be around for long? What's a question you wish people would ask more often?</t>
+  </si>
+  <si>
+    <t>What is the saddest thing about your life that nobody knows?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are you most sentimental about? </t>
+  </si>
+  <si>
+    <t>Do you think people more people look down on you or up to you? Why? What question do you most want an answer to?</t>
+  </si>
+  <si>
+    <t>What are some of the telltale signs of a shallow person?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What do you look forward to most in the day? </t>
+  </si>
+  <si>
+    <t>If you could instantly learn a talent or skill, what would you want to know how to do? When is your favorite time of day?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are the best and worst things about the period of history we are living through? What's the most rewarding thing in your daily routine? </t>
+  </si>
+  <si>
+    <t>What weird thing stresses you out more than it should?</t>
+  </si>
+  <si>
+    <t>When do you feel like you are really in your element?</t>
+  </si>
+  <si>
+    <t>How likely are you to believe in conspiracy theories?</t>
+  </si>
+  <si>
+    <t>What are some alcohol-induced stories of your younger days?</t>
+  </si>
+  <si>
+    <t>What's the best way for someone to improve themselves?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What was the most productive time in your life? How about the least productive? What three words best describe you? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How well do you function under a lot of pressure? What is your weakness? </t>
+  </si>
+  <si>
+    <t>What are two of the most important events in your life?</t>
+  </si>
+  <si>
+    <t>What is something you know is bad for you but you can't seem to get away from it?</t>
+  </si>
+  <si>
+    <t>What's the biggest favor you've done for someone?</t>
+  </si>
+  <si>
+    <t>How does your current morning routine compare to your ideal morning routine?</t>
+  </si>
+  <si>
+    <t>What brings you the most joy?</t>
+  </si>
+  <si>
+    <t>What are you purposefully ignoring even though you know you should probably deal with it?</t>
+  </si>
+  <si>
+    <t>What do you wish you were better at?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there anything you did wrong for years and years, only to discover later that you were doing it wrong? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is something your parents did or used to do that really embarrassed you? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What small seemingly insignificant thing did your parents, or someone else say when you were a child that has stuck with you all this time? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the best or worst thing you inherited from your parents? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What made you realize that your parents were just human like everyone else? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What habits do you still have from childhood? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What family vacations did you take as a child? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How traditionally “normal” was your family? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Children are often very similar to their parents. How do you want to be different than your parents? And how do you want to be similar to them? </t>
+  </si>
+  <si>
+    <t>What school subjects did you like and hate most when you were in school? What unique game of pretend did you frequently play as a child?</t>
+  </si>
+  <si>
+    <t>What movie seriously scarred you as a child or as an adult?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What irrational fears did you have as a child? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What toy played the most significant part in your childhood? What are some of your earliest memories? </t>
+  </si>
+  <si>
+    <t>What is something I did that you thought was exceptionally kind or thoughtful? What new hobbies or activities would you like to try together as a couple? What's our greatest strength as a couple?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What could we do to make our relationship stronger? </t>
+  </si>
+  <si>
+    <t>What is something small that we can do daily for each other to make our lives better? How much space / alone time should people in a relationship give each other?</t>
+  </si>
+  <si>
+    <t>What questions should partners ask each other before getting married?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What do I do that makes you the happiest? </t>
+  </si>
+  <si>
+    <t>How important is it for individuals in a relationship to maintain their own separate identity? What makes our relationship better than other relationships?</t>
+  </si>
+  <si>
+    <t>What do you think our life will look like in 10 years?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What do you think would bring us closer together as a couple? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What kind of memories do you want to make together? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What do you think the most essential thing in a successful relationship is? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What's your favorite way we spend time together? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What's your favorite gift I've given you? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Where do you want to live when we retire? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In what areas do you think our personalities complement each other? (i.e. One is too reckless, and the other is too cautious, and it balances out to a happy medium.) </t>
+  </si>
+  <si>
+    <t>How well do you think we communicate?</t>
+  </si>
+  <si>
+    <t>What adventure would you like to go on with me?</t>
+  </si>
+  <si>
+    <t>What's the best relationship advice you've received?</t>
+  </si>
+  <si>
+    <t>What are some things you really like about me?</t>
+  </si>
+  <si>
+    <t>What do you think the hardest thing about marriage/being in a relationship is? What can I do to most help us?</t>
+  </si>
+  <si>
+    <t>What do you see as your role in our relationship?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What would be a deal breaker for our relationship, something you couldn't forgive? </t>
+  </si>
+  <si>
+    <t>What makes us different than other couples?</t>
+  </si>
+  <si>
+    <t>What do you think would be the best way to strengthen our relationship? What are some of your relationship goals?</t>
+  </si>
+  <si>
+    <t>How realistic do you think couples in movies and TV are?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What does a happy and healthy relationship look like to you? </t>
+  </si>
+  <si>
+    <t>How well do you think our sex drives match up?</t>
+  </si>
+  <si>
+    <t>How important do you think sex is in our relationship?</t>
+  </si>
+  <si>
+    <t>What are you into, but haven’t told me about?</t>
+  </si>
+  <si>
+    <t>What do I do in bed that drives you wild?</t>
+  </si>
+  <si>
+    <t>What is the most adventurous thing you've done sexually?</t>
+  </si>
+  <si>
+    <t>Besides orgasms, what is the best part of sex?</t>
+  </si>
+  <si>
+    <t>What’s the most embarrassing thing that has happened to you while having sex? When am I at my sexiest?</t>
+  </si>
+  <si>
+    <t>What would you like me to do in the bedroom to spice things up a bit?</t>
+  </si>
+  <si>
+    <t>What’s better than great sex?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What do I do outside the bedroom that turns you on? </t>
+  </si>
+  <si>
+    <t>Do you eventually want to have children? How many children do you eventually want? Why? What's the worst parenting mistake a couple can make?</t>
+  </si>
+  <si>
+    <t>What is the best way to raise children?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How would we know if we did our job as parents well? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you think it is more important for a couple with kids to focus on the kids more or each other more? Why? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How do you think having kids will / has changed our lives and relationship? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether you are a new couple, or you've been a couple for years and years,
+we've got loads of questions for couples that will be perfect for getting a
+great conversation going. Level 1 is about ice breakers, Level 2 is about
+family and childhood, Level 3 is about relationship, and Level 4 is about
+sex and having kids. </t>
+  </si>
+  <si>
+    <t>Relationship Edition</t>
   </si>
 </sst>
 </file>
@@ -3507,6 +4048,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="page1image23251392">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00A916F2-4BFD-7E54-AADC-A816E4054A63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1651000" y="4953000"/>
+          <a:ext cx="3060700" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7912,7 +8519,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="A6" sqref="A6:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10441,9 +11048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266716F5-2382-4BA3-89BC-34C748FDC5CA}">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -10463,11 +11068,11 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>992</v>
       </c>
     </row>
@@ -10939,9 +11544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EB6A34-6766-4F36-ABD4-63EFDDDDD80E}">
   <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView zoomScale="158" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -11622,6 +12225,1970 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA8A9E1-0154-BF46-81F5-4F5B0654000C}">
+  <dimension ref="A1:C179"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>733</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>733</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>733</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>733</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>733</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>733</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>733</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>733</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>733</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>733</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>733</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>733</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>733</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>733</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>733</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>733</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>733</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>733</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>733</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>733</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>733</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>733</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>733</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>733</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>733</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>733</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>733</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>733</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>733</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>733</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>733</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>733</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>733</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>733</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>733</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>733</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>733</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>733</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>733</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>733</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>733</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>733</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>733</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>733</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>733</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52" t="s">
+        <v>733</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53" t="s">
+        <v>733</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
+        <v>733</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55" t="s">
+        <v>733</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56" t="s">
+        <v>733</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57" t="s">
+        <v>733</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58" t="s">
+        <v>733</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
+        <v>733</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60" t="s">
+        <v>733</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61" t="s">
+        <v>733</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>733</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>733</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64" t="s">
+        <v>733</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65" t="s">
+        <v>733</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66" t="s">
+        <v>733</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67" t="s">
+        <v>733</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>1</v>
+      </c>
+      <c r="B68" t="s">
+        <v>733</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>1</v>
+      </c>
+      <c r="B69" t="s">
+        <v>733</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>1</v>
+      </c>
+      <c r="B70" t="s">
+        <v>733</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>1</v>
+      </c>
+      <c r="B71" t="s">
+        <v>733</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>1</v>
+      </c>
+      <c r="B72" t="s">
+        <v>733</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>1</v>
+      </c>
+      <c r="B73" t="s">
+        <v>733</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="B74" t="s">
+        <v>733</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>1</v>
+      </c>
+      <c r="B75" t="s">
+        <v>733</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>1</v>
+      </c>
+      <c r="B76" t="s">
+        <v>733</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>1</v>
+      </c>
+      <c r="B77" t="s">
+        <v>733</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>1</v>
+      </c>
+      <c r="B78" t="s">
+        <v>733</v>
+      </c>
+      <c r="C78" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>1</v>
+      </c>
+      <c r="B79" t="s">
+        <v>733</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>1</v>
+      </c>
+      <c r="B80" t="s">
+        <v>733</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>1</v>
+      </c>
+      <c r="B81" t="s">
+        <v>733</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>1</v>
+      </c>
+      <c r="B82" t="s">
+        <v>733</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>1</v>
+      </c>
+      <c r="B83" t="s">
+        <v>733</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>1</v>
+      </c>
+      <c r="B84" t="s">
+        <v>733</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>1</v>
+      </c>
+      <c r="B85" t="s">
+        <v>733</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>1</v>
+      </c>
+      <c r="B86" t="s">
+        <v>733</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>1</v>
+      </c>
+      <c r="B87" t="s">
+        <v>733</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>1</v>
+      </c>
+      <c r="B88" t="s">
+        <v>733</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>1</v>
+      </c>
+      <c r="B89" t="s">
+        <v>733</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>1</v>
+      </c>
+      <c r="B90" t="s">
+        <v>733</v>
+      </c>
+      <c r="C90" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>1</v>
+      </c>
+      <c r="B91" t="s">
+        <v>733</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>1</v>
+      </c>
+      <c r="B92" t="s">
+        <v>733</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>1</v>
+      </c>
+      <c r="B93" t="s">
+        <v>733</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>1</v>
+      </c>
+      <c r="B94" t="s">
+        <v>733</v>
+      </c>
+      <c r="C94" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>1</v>
+      </c>
+      <c r="B95" t="s">
+        <v>733</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>1</v>
+      </c>
+      <c r="B96" t="s">
+        <v>733</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>1</v>
+      </c>
+      <c r="B97" t="s">
+        <v>733</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>1</v>
+      </c>
+      <c r="B98" t="s">
+        <v>733</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>1</v>
+      </c>
+      <c r="B99" t="s">
+        <v>733</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>1</v>
+      </c>
+      <c r="B100" t="s">
+        <v>733</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>1</v>
+      </c>
+      <c r="B101" t="s">
+        <v>733</v>
+      </c>
+      <c r="C101" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>1</v>
+      </c>
+      <c r="B102" t="s">
+        <v>733</v>
+      </c>
+      <c r="C102" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>1</v>
+      </c>
+      <c r="B103" t="s">
+        <v>733</v>
+      </c>
+      <c r="C103" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>1</v>
+      </c>
+      <c r="B104" t="s">
+        <v>733</v>
+      </c>
+      <c r="C104" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>1</v>
+      </c>
+      <c r="B105" t="s">
+        <v>733</v>
+      </c>
+      <c r="C105" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>1</v>
+      </c>
+      <c r="B106" t="s">
+        <v>733</v>
+      </c>
+      <c r="C106" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>1</v>
+      </c>
+      <c r="B107" t="s">
+        <v>733</v>
+      </c>
+      <c r="C107" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>1</v>
+      </c>
+      <c r="B108" t="s">
+        <v>733</v>
+      </c>
+      <c r="C108" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>1</v>
+      </c>
+      <c r="B109" t="s">
+        <v>733</v>
+      </c>
+      <c r="C109" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>1</v>
+      </c>
+      <c r="B110" t="s">
+        <v>733</v>
+      </c>
+      <c r="C110" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>1</v>
+      </c>
+      <c r="B111" t="s">
+        <v>733</v>
+      </c>
+      <c r="C111" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>1</v>
+      </c>
+      <c r="B112" t="s">
+        <v>733</v>
+      </c>
+      <c r="C112" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>1</v>
+      </c>
+      <c r="B113" t="s">
+        <v>733</v>
+      </c>
+      <c r="C113" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>1</v>
+      </c>
+      <c r="B114" t="s">
+        <v>733</v>
+      </c>
+      <c r="C114" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>1</v>
+      </c>
+      <c r="B115" t="s">
+        <v>733</v>
+      </c>
+      <c r="C115" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>1</v>
+      </c>
+      <c r="B116" t="s">
+        <v>733</v>
+      </c>
+      <c r="C116" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>1</v>
+      </c>
+      <c r="B117" t="s">
+        <v>733</v>
+      </c>
+      <c r="C117" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>1</v>
+      </c>
+      <c r="B118" t="s">
+        <v>733</v>
+      </c>
+      <c r="C118" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>1</v>
+      </c>
+      <c r="B119" t="s">
+        <v>733</v>
+      </c>
+      <c r="C119" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>1</v>
+      </c>
+      <c r="B120" t="s">
+        <v>733</v>
+      </c>
+      <c r="C120" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>1</v>
+      </c>
+      <c r="B121" t="s">
+        <v>733</v>
+      </c>
+      <c r="C121" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>1</v>
+      </c>
+      <c r="B122" t="s">
+        <v>733</v>
+      </c>
+      <c r="C122" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>1</v>
+      </c>
+      <c r="B123" t="s">
+        <v>733</v>
+      </c>
+      <c r="C123" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>1</v>
+      </c>
+      <c r="B124" t="s">
+        <v>733</v>
+      </c>
+      <c r="C124" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>1</v>
+      </c>
+      <c r="B125" t="s">
+        <v>733</v>
+      </c>
+      <c r="C125" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>1</v>
+      </c>
+      <c r="B126" t="s">
+        <v>733</v>
+      </c>
+      <c r="C126" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>1</v>
+      </c>
+      <c r="B127" t="s">
+        <v>733</v>
+      </c>
+      <c r="C127" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>2</v>
+      </c>
+      <c r="B128" t="s">
+        <v>758</v>
+      </c>
+      <c r="C128" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>2</v>
+      </c>
+      <c r="B129" t="s">
+        <v>758</v>
+      </c>
+      <c r="C129" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>2</v>
+      </c>
+      <c r="B130" t="s">
+        <v>758</v>
+      </c>
+      <c r="C130" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>2</v>
+      </c>
+      <c r="B131" t="s">
+        <v>758</v>
+      </c>
+      <c r="C131" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>2</v>
+      </c>
+      <c r="B132" t="s">
+        <v>758</v>
+      </c>
+      <c r="C132" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>2</v>
+      </c>
+      <c r="B133" t="s">
+        <v>758</v>
+      </c>
+      <c r="C133" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>2</v>
+      </c>
+      <c r="B134" t="s">
+        <v>758</v>
+      </c>
+      <c r="C134" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>2</v>
+      </c>
+      <c r="B135" t="s">
+        <v>758</v>
+      </c>
+      <c r="C135" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>2</v>
+      </c>
+      <c r="B136" t="s">
+        <v>758</v>
+      </c>
+      <c r="C136" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>2</v>
+      </c>
+      <c r="B137" t="s">
+        <v>758</v>
+      </c>
+      <c r="C137" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>2</v>
+      </c>
+      <c r="B138" t="s">
+        <v>758</v>
+      </c>
+      <c r="C138" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>2</v>
+      </c>
+      <c r="B139" t="s">
+        <v>758</v>
+      </c>
+      <c r="C139" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>3</v>
+      </c>
+      <c r="B140" t="s">
+        <v>3</v>
+      </c>
+      <c r="C140" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>3</v>
+      </c>
+      <c r="B141" t="s">
+        <v>3</v>
+      </c>
+      <c r="C141" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>3</v>
+      </c>
+      <c r="B142" t="s">
+        <v>3</v>
+      </c>
+      <c r="C142" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>3</v>
+      </c>
+      <c r="B143" t="s">
+        <v>3</v>
+      </c>
+      <c r="C143" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>3</v>
+      </c>
+      <c r="B144" t="s">
+        <v>3</v>
+      </c>
+      <c r="C144" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>3</v>
+      </c>
+      <c r="B145" t="s">
+        <v>3</v>
+      </c>
+      <c r="C145" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>3</v>
+      </c>
+      <c r="B146" t="s">
+        <v>3</v>
+      </c>
+      <c r="C146" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>3</v>
+      </c>
+      <c r="B147" t="s">
+        <v>3</v>
+      </c>
+      <c r="C147" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>3</v>
+      </c>
+      <c r="B148" t="s">
+        <v>3</v>
+      </c>
+      <c r="C148" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>3</v>
+      </c>
+      <c r="B149" t="s">
+        <v>3</v>
+      </c>
+      <c r="C149" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>3</v>
+      </c>
+      <c r="B150" t="s">
+        <v>3</v>
+      </c>
+      <c r="C150" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>3</v>
+      </c>
+      <c r="B151" t="s">
+        <v>3</v>
+      </c>
+      <c r="C151" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>3</v>
+      </c>
+      <c r="B152" t="s">
+        <v>3</v>
+      </c>
+      <c r="C152" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>3</v>
+      </c>
+      <c r="B153" t="s">
+        <v>3</v>
+      </c>
+      <c r="C153" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>3</v>
+      </c>
+      <c r="B154" t="s">
+        <v>3</v>
+      </c>
+      <c r="C154" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>3</v>
+      </c>
+      <c r="B155" t="s">
+        <v>3</v>
+      </c>
+      <c r="C155" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>3</v>
+      </c>
+      <c r="B156" t="s">
+        <v>3</v>
+      </c>
+      <c r="C156" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>3</v>
+      </c>
+      <c r="B157" t="s">
+        <v>3</v>
+      </c>
+      <c r="C157" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>3</v>
+      </c>
+      <c r="B158" t="s">
+        <v>3</v>
+      </c>
+      <c r="C158" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>3</v>
+      </c>
+      <c r="B159" t="s">
+        <v>3</v>
+      </c>
+      <c r="C159" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>3</v>
+      </c>
+      <c r="B160" t="s">
+        <v>3</v>
+      </c>
+      <c r="C160" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>3</v>
+      </c>
+      <c r="B161" t="s">
+        <v>3</v>
+      </c>
+      <c r="C161" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>3</v>
+      </c>
+      <c r="B162" t="s">
+        <v>3</v>
+      </c>
+      <c r="C162" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>3</v>
+      </c>
+      <c r="B163" t="s">
+        <v>3</v>
+      </c>
+      <c r="C163" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>3</v>
+      </c>
+      <c r="B164" t="s">
+        <v>3</v>
+      </c>
+      <c r="C164" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>4</v>
+      </c>
+      <c r="B165" t="s">
+        <v>724</v>
+      </c>
+      <c r="C165" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>4</v>
+      </c>
+      <c r="B166" t="s">
+        <v>724</v>
+      </c>
+      <c r="C166" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>4</v>
+      </c>
+      <c r="B167" t="s">
+        <v>724</v>
+      </c>
+      <c r="C167" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>4</v>
+      </c>
+      <c r="B168" t="s">
+        <v>724</v>
+      </c>
+      <c r="C168" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>4</v>
+      </c>
+      <c r="B169" t="s">
+        <v>724</v>
+      </c>
+      <c r="C169" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>4</v>
+      </c>
+      <c r="B170" t="s">
+        <v>724</v>
+      </c>
+      <c r="C170" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>4</v>
+      </c>
+      <c r="B171" t="s">
+        <v>724</v>
+      </c>
+      <c r="C171" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>4</v>
+      </c>
+      <c r="B172" t="s">
+        <v>724</v>
+      </c>
+      <c r="C172" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>4</v>
+      </c>
+      <c r="B173" t="s">
+        <v>724</v>
+      </c>
+      <c r="C173" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>4</v>
+      </c>
+      <c r="B174" t="s">
+        <v>724</v>
+      </c>
+      <c r="C174" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>4</v>
+      </c>
+      <c r="B175" t="s">
+        <v>724</v>
+      </c>
+      <c r="C175" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>4</v>
+      </c>
+      <c r="B176" t="s">
+        <v>724</v>
+      </c>
+      <c r="C176" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>4</v>
+      </c>
+      <c r="B177" t="s">
+        <v>724</v>
+      </c>
+      <c r="C177" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>4</v>
+      </c>
+      <c r="B178" t="s">
+        <v>724</v>
+      </c>
+      <c r="C178" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>4</v>
+      </c>
+      <c r="B179" t="s">
+        <v>724</v>
+      </c>
+      <c r="C179" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12092,7 +14659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB304941-4562-46A1-BF92-E2BAD3F0C635}">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>

<commit_message>
clean up card game
</commit_message>
<xml_diff>
--- a/data/WNRS.xlsx
+++ b/data/WNRS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KayJan/test-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F4FB6B-67EE-5F46-B663-37E92BC85FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9BD564-8970-4B46-98A7-C6AF3064BE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-5320" windowWidth="38400" windowHeight="21100" tabRatio="829" firstSheet="12" activeTab="23" xr2:uid="{35520F66-FEA5-4575-927A-C3FC8E8C1344}"/>
+    <workbookView xWindow="-19200" yWindow="-5320" windowWidth="19200" windowHeight="21100" tabRatio="829" firstSheet="12" activeTab="23" xr2:uid="{35520F66-FEA5-4575-927A-C3FC8E8C1344}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Deck" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2665" uniqueCount="1275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2731" uniqueCount="1308">
   <si>
     <t>Card</t>
   </si>
@@ -3488,15 +3488,9 @@
     <t>What musical instrument do you wish you could play?</t>
   </si>
   <si>
-    <t>When has a mundane occurrence or chance completely changed the course of your life? What is the nicest compliment you've received?</t>
-  </si>
-  <si>
     <t>What age would you like to live to?</t>
   </si>
   <si>
-    <t>If you could travel to any country in the world for one month, where would you go? What is your favorite memory of someone who isn't in your life anymore?</t>
-  </si>
-  <si>
     <t>How superstitious are you?</t>
   </si>
   <si>
@@ -3521,12 +3515,6 @@
     <t xml:space="preserve">If you had a friend who spoke to you the same way you speak to yourself, would you keep them as a friend? </t>
   </si>
   <si>
-    <t>What petty thing that people do really gets on your nerves? What brings meaning to your life?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is something you wish you could say to people but can’t? What are some of the most attractive traits a person can have? What's a secret you've never told anyone? </t>
-  </si>
-  <si>
     <t>What small pleasures do you enjoy the most?</t>
   </si>
   <si>
@@ -3539,9 +3527,6 @@
     <t>What have you struggled with your entire life?</t>
   </si>
   <si>
-    <t xml:space="preserve">What is the most significant change you would like to make in your life? What do you want out of life? </t>
-  </si>
-  <si>
     <t>What calms you down the most?</t>
   </si>
   <si>
@@ -3566,9 +3551,6 @@
     <t>Who do you act nice around but secretly dislike?</t>
   </si>
   <si>
-    <t>If money was no object, and with no input from me, how would you decorate your / our house? How good are you at reading people?</t>
-  </si>
-  <si>
     <t>Are you hopeful about your future?</t>
   </si>
   <si>
@@ -3626,9 +3608,6 @@
     <t>What was the hardest lesson you’ve had to learn?</t>
   </si>
   <si>
-    <t>Would you take 3 million dollars if it meant that the person you hate most in the world gets 9 million? What part of you as a person still needs a lot of work?</t>
-  </si>
-  <si>
     <t>What are some words of wisdom that have stuck with you all these years?</t>
   </si>
   <si>
@@ -3644,18 +3623,12 @@
     <t>Tell me about a time you almost died.</t>
   </si>
   <si>
-    <t>Are you ashamed of anything you did in the past? If you are comfortable talking about it, what was it? Do you prefer living in the countryside, in a town, or in a big city? Why?</t>
-  </si>
-  <si>
     <t>What's your fondest memory of a tree?</t>
   </si>
   <si>
     <t>What are some of the most pleasant sensations for you?</t>
   </si>
   <si>
-    <t>Are you happy with the career path you chose or do you wish you had chosen a different career? What's the most unethical thing you do regularly?</t>
-  </si>
-  <si>
     <t>What is way more difficult than it sounds?</t>
   </si>
   <si>
@@ -3716,9 +3689,6 @@
     <t>What animal are you most afraid of?</t>
   </si>
   <si>
-    <t xml:space="preserve">What scandal happened in your neighbor or town when you were growing up? How well do you think you would handle prison? </t>
-  </si>
-  <si>
     <t>What's the most awkward social situation you've been in?</t>
   </si>
   <si>
@@ -3731,51 +3701,27 @@
     <t>What's the most peaceful/restful night of sleep you've had?</t>
   </si>
   <si>
-    <t xml:space="preserve">What's the most dangerous, thrill-seeking thing you would consider doing? What's your biggest regret? </t>
-  </si>
-  <si>
     <t xml:space="preserve">Is it better to trust people or not trust people? And why? </t>
   </si>
   <si>
-    <t>What do you think your best and worst personality traits are? Who do you miss the most?</t>
-  </si>
-  <si>
     <t>What is the hardest life lesson you've had to learn?</t>
   </si>
   <si>
     <t xml:space="preserve">What do you take for granted? </t>
   </si>
   <si>
-    <t>What's the most stressful situation you've been in? How did you handle it? What's the most ambitious thing you've attempted?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How often do you change your opinions or how you view the world? What's the biggest opportunity you were given? </t>
-  </si>
-  <si>
-    <t>What is something we should enjoy more because it won't be around for long? What's a question you wish people would ask more often?</t>
-  </si>
-  <si>
     <t>What is the saddest thing about your life that nobody knows?</t>
   </si>
   <si>
     <t xml:space="preserve">What are you most sentimental about? </t>
   </si>
   <si>
-    <t>Do you think people more people look down on you or up to you? Why? What question do you most want an answer to?</t>
-  </si>
-  <si>
     <t>What are some of the telltale signs of a shallow person?</t>
   </si>
   <si>
     <t xml:space="preserve">What do you look forward to most in the day? </t>
   </si>
   <si>
-    <t>If you could instantly learn a talent or skill, what would you want to know how to do? When is your favorite time of day?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What are the best and worst things about the period of history we are living through? What's the most rewarding thing in your daily routine? </t>
-  </si>
-  <si>
     <t>What weird thing stresses you out more than it should?</t>
   </si>
   <si>
@@ -3791,12 +3737,6 @@
     <t>What's the best way for someone to improve themselves?</t>
   </si>
   <si>
-    <t xml:space="preserve">What was the most productive time in your life? How about the least productive? What three words best describe you? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">How well do you function under a lot of pressure? What is your weakness? </t>
-  </si>
-  <si>
     <t>What are two of the most important events in your life?</t>
   </si>
   <si>
@@ -3845,36 +3785,21 @@
     <t xml:space="preserve">Children are often very similar to their parents. How do you want to be different than your parents? And how do you want to be similar to them? </t>
   </si>
   <si>
-    <t>What school subjects did you like and hate most when you were in school? What unique game of pretend did you frequently play as a child?</t>
-  </si>
-  <si>
     <t>What movie seriously scarred you as a child or as an adult?</t>
   </si>
   <si>
     <t xml:space="preserve">What irrational fears did you have as a child? </t>
   </si>
   <si>
-    <t xml:space="preserve">What toy played the most significant part in your childhood? What are some of your earliest memories? </t>
-  </si>
-  <si>
-    <t>What is something I did that you thought was exceptionally kind or thoughtful? What new hobbies or activities would you like to try together as a couple? What's our greatest strength as a couple?</t>
-  </si>
-  <si>
     <t xml:space="preserve">What could we do to make our relationship stronger? </t>
   </si>
   <si>
-    <t>What is something small that we can do daily for each other to make our lives better? How much space / alone time should people in a relationship give each other?</t>
-  </si>
-  <si>
     <t>What questions should partners ask each other before getting married?</t>
   </si>
   <si>
     <t xml:space="preserve">What do I do that makes you the happiest? </t>
   </si>
   <si>
-    <t>How important is it for individuals in a relationship to maintain their own separate identity? What makes our relationship better than other relationships?</t>
-  </si>
-  <si>
     <t>What do you think our life will look like in 10 years?</t>
   </si>
   <si>
@@ -3911,9 +3836,6 @@
     <t>What are some things you really like about me?</t>
   </si>
   <si>
-    <t>What do you think the hardest thing about marriage/being in a relationship is? What can I do to most help us?</t>
-  </si>
-  <si>
     <t>What do you see as your role in our relationship?</t>
   </si>
   <si>
@@ -3923,9 +3845,6 @@
     <t>What makes us different than other couples?</t>
   </si>
   <si>
-    <t>What do you think would be the best way to strengthen our relationship? What are some of your relationship goals?</t>
-  </si>
-  <si>
     <t>How realistic do you think couples in movies and TV are?</t>
   </si>
   <si>
@@ -3950,9 +3869,6 @@
     <t>Besides orgasms, what is the best part of sex?</t>
   </si>
   <si>
-    <t>What’s the most embarrassing thing that has happened to you while having sex? When am I at my sexiest?</t>
-  </si>
-  <si>
     <t>What would you like me to do in the bedroom to spice things up a bit?</t>
   </si>
   <si>
@@ -3960,9 +3876,6 @@
   </si>
   <si>
     <t xml:space="preserve">What do I do outside the bedroom that turns you on? </t>
-  </si>
-  <si>
-    <t>Do you eventually want to have children? How many children do you eventually want? Why? What's the worst parenting mistake a couple can make?</t>
   </si>
   <si>
     <t>What is the best way to raise children?</t>
@@ -3985,6 +3898,192 @@
   </si>
   <si>
     <t>Relationship Edition</t>
+  </si>
+  <si>
+    <t>What is the nicest compliment you’ve received?</t>
+  </si>
+  <si>
+    <t>When has a mundane occurrence or chance completely changed the course of your life?</t>
+  </si>
+  <si>
+    <t>If you could travel to any country in the world for one month, where would you go?</t>
+  </si>
+  <si>
+    <t>What is your favorite memory of someone who isn't in your life anymore?</t>
+  </si>
+  <si>
+    <t>What is something you wish you could say to people but can’t?</t>
+  </si>
+  <si>
+    <t>What are some of the most attractive traits a person can have?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What's a secret you've never told anyone? </t>
+  </si>
+  <si>
+    <t>If money was no object, and with no input from me, how would you decorate your / our house?</t>
+  </si>
+  <si>
+    <t>How good are you at reading people?</t>
+  </si>
+  <si>
+    <t>Would you take 3 million dollars if it meant that the person you hate most in the world gets 9 million?</t>
+  </si>
+  <si>
+    <t>What part of you as a person still needs a lot of work?</t>
+  </si>
+  <si>
+    <t>Are you ashamed of anything you did in the past? If you are comfortable talking about it, what was it?</t>
+  </si>
+  <si>
+    <t>Do you prefer living in the countryside, in a town, or in a big city? Why?</t>
+  </si>
+  <si>
+    <t>Are you happy with the career path you chose or do you wish you had chosen a different career?</t>
+  </si>
+  <si>
+    <t>What's the most unethical thing you do regularly?</t>
+  </si>
+  <si>
+    <t>What scandal happened in your neighbor or town when you were growing up?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How well do you think you would handle prison? </t>
+  </si>
+  <si>
+    <t>What's the most dangerous, thrill-seeking thing you would consider doing?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What's your biggest regret? </t>
+  </si>
+  <si>
+    <t>What do you think your best and worst personality traits are?</t>
+  </si>
+  <si>
+    <t>Who do you miss the most?</t>
+  </si>
+  <si>
+    <t>What's the most stressful situation you've been in? How did you handle it?</t>
+  </si>
+  <si>
+    <t>What's the most ambitious thing you've attempted?</t>
+  </si>
+  <si>
+    <t>How often do you change your opinions or how you view the world?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What's the biggest opportunity you were given? </t>
+  </si>
+  <si>
+    <t>What is something we should enjoy more because it won't be around for long?</t>
+  </si>
+  <si>
+    <t>What's a question you wish people would ask more often?</t>
+  </si>
+  <si>
+    <t>Do you think people more people look down on you or up to you? Why?</t>
+  </si>
+  <si>
+    <t>What question do you most want an answer to?</t>
+  </si>
+  <si>
+    <t>If you could instantly learn a talent or skill, what would you want to know how to do?</t>
+  </si>
+  <si>
+    <t>When is your favorite time of day?</t>
+  </si>
+  <si>
+    <t>What are the best and worst things about the period of history we are living through?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What's the most rewarding thing in your daily routine? </t>
+  </si>
+  <si>
+    <t>What was the most productive time in your life? How about the least productive?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What three words best describe you? </t>
+  </si>
+  <si>
+    <t>What's the worst parenting mistake a couple can make?</t>
+  </si>
+  <si>
+    <t>What do you think would be the best way to strengthen our relationship?</t>
+  </si>
+  <si>
+    <t>What are some of your relationship goals?</t>
+  </si>
+  <si>
+    <t>How important is it for individuals in a relationship to maintain their own separate identity?</t>
+  </si>
+  <si>
+    <t>What makes our relationship better than other relationships?</t>
+  </si>
+  <si>
+    <t>What is something small that we can do daily for each other to make our lives better?</t>
+  </si>
+  <si>
+    <t>How much space / alone time should people in a relationship give each other?</t>
+  </si>
+  <si>
+    <t>What is something I did that you thought was exceptionally kind or thoughtful?</t>
+  </si>
+  <si>
+    <t>What new hobbies or activities would you like to try together as a couple?</t>
+  </si>
+  <si>
+    <t>What's our greatest strength as a couple?</t>
+  </si>
+  <si>
+    <t>How well do you function under a lot of pressure?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is your weakness? </t>
+  </si>
+  <si>
+    <t>What school subjects did you like and hate most when you were in school?</t>
+  </si>
+  <si>
+    <t>What unique game of pretend did you frequently play as a child?</t>
+  </si>
+  <si>
+    <t>What toy played the most significant part in your childhood?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are some of your earliest memories? </t>
+  </si>
+  <si>
+    <t>What petty thing that people do really gets on your nerves?</t>
+  </si>
+  <si>
+    <t>What brings meaning to your life?</t>
+  </si>
+  <si>
+    <t>What is the most significant change you would like to make in your life?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What do you want out of life? </t>
+  </si>
+  <si>
+    <t>What does your perfect date look like?</t>
+  </si>
+  <si>
+    <t>How often would you like to go out on a date?</t>
+  </si>
+  <si>
+    <t>What do you think the hardest thing about marriage/being in a relationship is?</t>
+  </si>
+  <si>
+    <t>What can I do to most help us?</t>
+  </si>
+  <si>
+    <t>What’s the most embarrassing thing that has happened to you while having sex?</t>
+  </si>
+  <si>
+    <t>When am I at my sexiest?</t>
+  </si>
+  <si>
+    <t>Do you eventually want to have children? How many children do you eventually want? Why?</t>
   </si>
 </sst>
 </file>
@@ -4056,13 +4155,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4093,7 +4192,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1651000" y="4953000"/>
+          <a:off x="1651000" y="5334000"/>
           <a:ext cx="3060700" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12230,7 +12329,7 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA8A9E1-0154-BF46-81F5-4F5B0654000C}">
-  <dimension ref="A1:C179"/>
+  <dimension ref="A1:C212"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0"/>
   </sheetViews>
@@ -12249,7 +12348,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>1274</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -12257,7 +12356,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1273</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -12400,7 +12499,7 @@
         <v>733</v>
       </c>
       <c r="C17" t="s">
-        <v>1110</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -12411,7 +12510,7 @@
         <v>733</v>
       </c>
       <c r="C18" t="s">
-        <v>1111</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -12422,7 +12521,7 @@
         <v>733</v>
       </c>
       <c r="C19" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -12433,7 +12532,7 @@
         <v>733</v>
       </c>
       <c r="C20" t="s">
-        <v>1113</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -12444,7 +12543,7 @@
         <v>733</v>
       </c>
       <c r="C21" t="s">
-        <v>1114</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -12455,7 +12554,7 @@
         <v>733</v>
       </c>
       <c r="C22" t="s">
-        <v>1115</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -12466,7 +12565,7 @@
         <v>733</v>
       </c>
       <c r="C23" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -12477,7 +12576,7 @@
         <v>733</v>
       </c>
       <c r="C24" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -12488,7 +12587,7 @@
         <v>733</v>
       </c>
       <c r="C25" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -12499,7 +12598,7 @@
         <v>733</v>
       </c>
       <c r="C26" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -12510,7 +12609,7 @@
         <v>733</v>
       </c>
       <c r="C27" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -12521,7 +12620,7 @@
         <v>733</v>
       </c>
       <c r="C28" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -12532,7 +12631,7 @@
         <v>733</v>
       </c>
       <c r="C29" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -12543,7 +12642,7 @@
         <v>733</v>
       </c>
       <c r="C30" t="s">
-        <v>1123</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -12554,7 +12653,7 @@
         <v>733</v>
       </c>
       <c r="C31" t="s">
-        <v>1124</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -12565,7 +12664,7 @@
         <v>733</v>
       </c>
       <c r="C32" t="s">
-        <v>1125</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -12576,7 +12675,7 @@
         <v>733</v>
       </c>
       <c r="C33" t="s">
-        <v>1126</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -12587,7 +12686,7 @@
         <v>733</v>
       </c>
       <c r="C34" t="s">
-        <v>1127</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -12598,7 +12697,7 @@
         <v>733</v>
       </c>
       <c r="C35" t="s">
-        <v>1128</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -12609,7 +12708,7 @@
         <v>733</v>
       </c>
       <c r="C36" t="s">
-        <v>1129</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -12620,7 +12719,7 @@
         <v>733</v>
       </c>
       <c r="C37" t="s">
-        <v>1130</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -12631,7 +12730,7 @@
         <v>733</v>
       </c>
       <c r="C38" t="s">
-        <v>1131</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -12642,7 +12741,7 @@
         <v>733</v>
       </c>
       <c r="C39" t="s">
-        <v>1132</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -12653,7 +12752,7 @@
         <v>733</v>
       </c>
       <c r="C40" t="s">
-        <v>1133</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -12664,7 +12763,7 @@
         <v>733</v>
       </c>
       <c r="C41" t="s">
-        <v>1134</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -12675,7 +12774,7 @@
         <v>733</v>
       </c>
       <c r="C42" t="s">
-        <v>1135</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -12686,7 +12785,7 @@
         <v>733</v>
       </c>
       <c r="C43" t="s">
-        <v>1136</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -12697,7 +12796,7 @@
         <v>733</v>
       </c>
       <c r="C44" t="s">
-        <v>1137</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -12708,7 +12807,7 @@
         <v>733</v>
       </c>
       <c r="C45" t="s">
-        <v>1138</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -12719,7 +12818,7 @@
         <v>733</v>
       </c>
       <c r="C46" t="s">
-        <v>1139</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -12730,7 +12829,7 @@
         <v>733</v>
       </c>
       <c r="C47" t="s">
-        <v>1140</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -12741,7 +12840,7 @@
         <v>733</v>
       </c>
       <c r="C48" t="s">
-        <v>1141</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -12752,7 +12851,7 @@
         <v>733</v>
       </c>
       <c r="C49" t="s">
-        <v>1142</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -12763,7 +12862,7 @@
         <v>733</v>
       </c>
       <c r="C50" t="s">
-        <v>1143</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -12774,7 +12873,7 @@
         <v>733</v>
       </c>
       <c r="C51" t="s">
-        <v>1144</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -12785,7 +12884,7 @@
         <v>733</v>
       </c>
       <c r="C52" t="s">
-        <v>1145</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -12796,7 +12895,7 @@
         <v>733</v>
       </c>
       <c r="C53" t="s">
-        <v>1146</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -12807,7 +12906,7 @@
         <v>733</v>
       </c>
       <c r="C54" t="s">
-        <v>1147</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -12818,7 +12917,7 @@
         <v>733</v>
       </c>
       <c r="C55" t="s">
-        <v>1148</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -12829,7 +12928,7 @@
         <v>733</v>
       </c>
       <c r="C56" t="s">
-        <v>1149</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -12840,7 +12939,7 @@
         <v>733</v>
       </c>
       <c r="C57" t="s">
-        <v>1150</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -12851,7 +12950,7 @@
         <v>733</v>
       </c>
       <c r="C58" t="s">
-        <v>1151</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -12862,7 +12961,7 @@
         <v>733</v>
       </c>
       <c r="C59" t="s">
-        <v>1152</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -12873,7 +12972,7 @@
         <v>733</v>
       </c>
       <c r="C60" t="s">
-        <v>1153</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -12884,7 +12983,7 @@
         <v>733</v>
       </c>
       <c r="C61" t="s">
-        <v>1154</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -12895,7 +12994,7 @@
         <v>733</v>
       </c>
       <c r="C62" t="s">
-        <v>1155</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -12906,7 +13005,7 @@
         <v>733</v>
       </c>
       <c r="C63" t="s">
-        <v>1156</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -12917,7 +13016,7 @@
         <v>733</v>
       </c>
       <c r="C64" t="s">
-        <v>1157</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -12928,7 +13027,7 @@
         <v>733</v>
       </c>
       <c r="C65" t="s">
-        <v>1158</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -12939,7 +13038,7 @@
         <v>733</v>
       </c>
       <c r="C66" t="s">
-        <v>1159</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -12950,7 +13049,7 @@
         <v>733</v>
       </c>
       <c r="C67" t="s">
-        <v>1160</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -12961,7 +13060,7 @@
         <v>733</v>
       </c>
       <c r="C68" t="s">
-        <v>1161</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -12972,7 +13071,7 @@
         <v>733</v>
       </c>
       <c r="C69" t="s">
-        <v>1162</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -12983,7 +13082,7 @@
         <v>733</v>
       </c>
       <c r="C70" t="s">
-        <v>1163</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -12994,7 +13093,7 @@
         <v>733</v>
       </c>
       <c r="C71" t="s">
-        <v>1164</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -13005,7 +13104,7 @@
         <v>733</v>
       </c>
       <c r="C72" t="s">
-        <v>1165</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -13016,7 +13115,7 @@
         <v>733</v>
       </c>
       <c r="C73" t="s">
-        <v>1166</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -13027,7 +13126,7 @@
         <v>733</v>
       </c>
       <c r="C74" t="s">
-        <v>1167</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -13038,7 +13137,7 @@
         <v>733</v>
       </c>
       <c r="C75" t="s">
-        <v>1168</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -13049,7 +13148,7 @@
         <v>733</v>
       </c>
       <c r="C76" t="s">
-        <v>1169</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -13060,7 +13159,7 @@
         <v>733</v>
       </c>
       <c r="C77" t="s">
-        <v>1170</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -13071,7 +13170,7 @@
         <v>733</v>
       </c>
       <c r="C78" t="s">
-        <v>1171</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -13082,7 +13181,7 @@
         <v>733</v>
       </c>
       <c r="C79" t="s">
-        <v>1172</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -13093,7 +13192,7 @@
         <v>733</v>
       </c>
       <c r="C80" t="s">
-        <v>1173</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -13104,7 +13203,7 @@
         <v>733</v>
       </c>
       <c r="C81" t="s">
-        <v>1174</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -13115,7 +13214,7 @@
         <v>733</v>
       </c>
       <c r="C82" t="s">
-        <v>1175</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -13126,7 +13225,7 @@
         <v>733</v>
       </c>
       <c r="C83" t="s">
-        <v>1176</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -13137,7 +13236,7 @@
         <v>733</v>
       </c>
       <c r="C84" t="s">
-        <v>1177</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -13148,7 +13247,7 @@
         <v>733</v>
       </c>
       <c r="C85" t="s">
-        <v>1178</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -13159,7 +13258,7 @@
         <v>733</v>
       </c>
       <c r="C86" t="s">
-        <v>1179</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -13170,7 +13269,7 @@
         <v>733</v>
       </c>
       <c r="C87" t="s">
-        <v>1180</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -13181,7 +13280,7 @@
         <v>733</v>
       </c>
       <c r="C88" t="s">
-        <v>1181</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -13192,7 +13291,7 @@
         <v>733</v>
       </c>
       <c r="C89" t="s">
-        <v>1182</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -13203,7 +13302,7 @@
         <v>733</v>
       </c>
       <c r="C90" t="s">
-        <v>1183</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -13214,7 +13313,7 @@
         <v>733</v>
       </c>
       <c r="C91" t="s">
-        <v>1184</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -13225,7 +13324,7 @@
         <v>733</v>
       </c>
       <c r="C92" t="s">
-        <v>1185</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -13236,7 +13335,7 @@
         <v>733</v>
       </c>
       <c r="C93" t="s">
-        <v>1186</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -13247,7 +13346,7 @@
         <v>733</v>
       </c>
       <c r="C94" t="s">
-        <v>1187</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -13258,7 +13357,7 @@
         <v>733</v>
       </c>
       <c r="C95" t="s">
-        <v>1188</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -13269,7 +13368,7 @@
         <v>733</v>
       </c>
       <c r="C96" t="s">
-        <v>1189</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -13280,7 +13379,7 @@
         <v>733</v>
       </c>
       <c r="C97" t="s">
-        <v>1190</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -13291,7 +13390,7 @@
         <v>733</v>
       </c>
       <c r="C98" t="s">
-        <v>1191</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -13302,7 +13401,7 @@
         <v>733</v>
       </c>
       <c r="C99" t="s">
-        <v>1192</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -13313,7 +13412,7 @@
         <v>733</v>
       </c>
       <c r="C100" t="s">
-        <v>1193</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -13324,7 +13423,7 @@
         <v>733</v>
       </c>
       <c r="C101" t="s">
-        <v>1194</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -13335,7 +13434,7 @@
         <v>733</v>
       </c>
       <c r="C102" t="s">
-        <v>1195</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -13346,7 +13445,7 @@
         <v>733</v>
       </c>
       <c r="C103" t="s">
-        <v>1196</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -13357,7 +13456,7 @@
         <v>733</v>
       </c>
       <c r="C104" t="s">
-        <v>1197</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -13368,7 +13467,7 @@
         <v>733</v>
       </c>
       <c r="C105" t="s">
-        <v>1198</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -13379,7 +13478,7 @@
         <v>733</v>
       </c>
       <c r="C106" t="s">
-        <v>1199</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -13390,7 +13489,7 @@
         <v>733</v>
       </c>
       <c r="C107" t="s">
-        <v>1200</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -13401,7 +13500,7 @@
         <v>733</v>
       </c>
       <c r="C108" t="s">
-        <v>1201</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -13412,7 +13511,7 @@
         <v>733</v>
       </c>
       <c r="C109" t="s">
-        <v>1202</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -13423,7 +13522,7 @@
         <v>733</v>
       </c>
       <c r="C110" t="s">
-        <v>1203</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -13434,7 +13533,7 @@
         <v>733</v>
       </c>
       <c r="C111" t="s">
-        <v>1204</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -13445,7 +13544,7 @@
         <v>733</v>
       </c>
       <c r="C112" t="s">
-        <v>1205</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -13456,7 +13555,7 @@
         <v>733</v>
       </c>
       <c r="C113" t="s">
-        <v>1206</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -13467,7 +13566,7 @@
         <v>733</v>
       </c>
       <c r="C114" t="s">
-        <v>1207</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -13478,7 +13577,7 @@
         <v>733</v>
       </c>
       <c r="C115" t="s">
-        <v>1208</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -13489,7 +13588,7 @@
         <v>733</v>
       </c>
       <c r="C116" t="s">
-        <v>1209</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -13500,7 +13599,7 @@
         <v>733</v>
       </c>
       <c r="C117" t="s">
-        <v>1210</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -13511,7 +13610,7 @@
         <v>733</v>
       </c>
       <c r="C118" t="s">
-        <v>1211</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -13522,7 +13621,7 @@
         <v>733</v>
       </c>
       <c r="C119" t="s">
-        <v>1212</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -13533,7 +13632,7 @@
         <v>733</v>
       </c>
       <c r="C120" t="s">
-        <v>1213</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -13544,7 +13643,7 @@
         <v>733</v>
       </c>
       <c r="C121" t="s">
-        <v>1214</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -13555,7 +13654,7 @@
         <v>733</v>
       </c>
       <c r="C122" t="s">
-        <v>1215</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
@@ -13566,7 +13665,7 @@
         <v>733</v>
       </c>
       <c r="C123" t="s">
-        <v>1216</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
@@ -13577,7 +13676,7 @@
         <v>733</v>
       </c>
       <c r="C124" t="s">
-        <v>1217</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
@@ -13588,7 +13687,7 @@
         <v>733</v>
       </c>
       <c r="C125" t="s">
-        <v>1218</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
@@ -13599,7 +13698,7 @@
         <v>733</v>
       </c>
       <c r="C126" t="s">
-        <v>1219</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
@@ -13610,403 +13709,403 @@
         <v>733</v>
       </c>
       <c r="C127" t="s">
-        <v>1220</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B128" t="s">
-        <v>758</v>
+        <v>733</v>
       </c>
       <c r="C128" t="s">
-        <v>1221</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B129" t="s">
-        <v>758</v>
+        <v>733</v>
       </c>
       <c r="C129" t="s">
-        <v>1222</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B130" t="s">
-        <v>758</v>
+        <v>733</v>
       </c>
       <c r="C130" t="s">
-        <v>1223</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B131" t="s">
-        <v>758</v>
+        <v>733</v>
       </c>
       <c r="C131" t="s">
-        <v>1224</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B132" t="s">
-        <v>758</v>
+        <v>733</v>
       </c>
       <c r="C132" t="s">
-        <v>1225</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B133" t="s">
-        <v>758</v>
+        <v>733</v>
       </c>
       <c r="C133" t="s">
-        <v>1226</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B134" t="s">
-        <v>758</v>
+        <v>733</v>
       </c>
       <c r="C134" t="s">
-        <v>1227</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B135" t="s">
-        <v>758</v>
+        <v>733</v>
       </c>
       <c r="C135" t="s">
-        <v>1228</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B136" t="s">
-        <v>758</v>
+        <v>733</v>
       </c>
       <c r="C136" t="s">
-        <v>1229</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B137" t="s">
-        <v>758</v>
+        <v>733</v>
       </c>
       <c r="C137" t="s">
-        <v>1230</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B138" t="s">
-        <v>758</v>
+        <v>733</v>
       </c>
       <c r="C138" t="s">
-        <v>1231</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B139" t="s">
-        <v>758</v>
+        <v>733</v>
       </c>
       <c r="C139" t="s">
-        <v>1232</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B140" t="s">
-        <v>3</v>
+        <v>733</v>
       </c>
       <c r="C140" t="s">
-        <v>1233</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B141" t="s">
-        <v>3</v>
+        <v>733</v>
       </c>
       <c r="C141" t="s">
-        <v>1234</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B142" t="s">
-        <v>3</v>
+        <v>733</v>
       </c>
       <c r="C142" t="s">
-        <v>1235</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B143" t="s">
-        <v>3</v>
+        <v>733</v>
       </c>
       <c r="C143" t="s">
-        <v>1236</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B144" t="s">
-        <v>3</v>
+        <v>733</v>
       </c>
       <c r="C144" t="s">
-        <v>1237</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B145" t="s">
-        <v>3</v>
+        <v>733</v>
       </c>
       <c r="C145" t="s">
-        <v>1238</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B146" t="s">
-        <v>3</v>
+        <v>733</v>
       </c>
       <c r="C146" t="s">
-        <v>1239</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B147" t="s">
-        <v>3</v>
+        <v>733</v>
       </c>
       <c r="C147" t="s">
-        <v>1240</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B148" t="s">
-        <v>3</v>
+        <v>733</v>
       </c>
       <c r="C148" t="s">
-        <v>1241</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B149" t="s">
-        <v>3</v>
+        <v>733</v>
       </c>
       <c r="C149" t="s">
-        <v>1242</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B150" t="s">
-        <v>3</v>
+        <v>758</v>
       </c>
       <c r="C150" t="s">
-        <v>1243</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B151" t="s">
-        <v>3</v>
+        <v>758</v>
       </c>
       <c r="C151" t="s">
-        <v>1244</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B152" t="s">
-        <v>3</v>
+        <v>758</v>
       </c>
       <c r="C152" t="s">
-        <v>1245</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B153" t="s">
-        <v>3</v>
+        <v>758</v>
       </c>
       <c r="C153" t="s">
-        <v>1246</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B154" t="s">
-        <v>3</v>
+        <v>758</v>
       </c>
       <c r="C154" t="s">
-        <v>1247</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B155" t="s">
-        <v>3</v>
+        <v>758</v>
       </c>
       <c r="C155" t="s">
-        <v>1248</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B156" t="s">
-        <v>3</v>
+        <v>758</v>
       </c>
       <c r="C156" t="s">
-        <v>1249</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B157" t="s">
-        <v>3</v>
+        <v>758</v>
       </c>
       <c r="C157" t="s">
-        <v>1250</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B158" t="s">
-        <v>3</v>
+        <v>758</v>
       </c>
       <c r="C158" t="s">
-        <v>1251</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B159" t="s">
-        <v>3</v>
+        <v>758</v>
       </c>
       <c r="C159" t="s">
-        <v>1252</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B160" t="s">
-        <v>3</v>
+        <v>758</v>
       </c>
       <c r="C160" t="s">
-        <v>1253</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B161" t="s">
-        <v>3</v>
+        <v>758</v>
       </c>
       <c r="C161" t="s">
-        <v>1254</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B162" t="s">
-        <v>3</v>
+        <v>758</v>
       </c>
       <c r="C162" t="s">
-        <v>1255</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B163" t="s">
-        <v>3</v>
+        <v>758</v>
       </c>
       <c r="C163" t="s">
-        <v>1256</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
@@ -14017,172 +14116,535 @@
         <v>3</v>
       </c>
       <c r="C164" t="s">
-        <v>1257</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B165" t="s">
-        <v>724</v>
+        <v>3</v>
       </c>
       <c r="C165" t="s">
-        <v>1258</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B166" t="s">
-        <v>724</v>
+        <v>3</v>
       </c>
       <c r="C166" t="s">
-        <v>1259</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B167" t="s">
-        <v>724</v>
+        <v>3</v>
       </c>
       <c r="C167" t="s">
-        <v>1260</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B168" t="s">
-        <v>724</v>
+        <v>3</v>
       </c>
       <c r="C168" t="s">
-        <v>1261</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B169" t="s">
-        <v>724</v>
+        <v>3</v>
       </c>
       <c r="C169" t="s">
-        <v>1262</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B170" t="s">
-        <v>724</v>
+        <v>3</v>
       </c>
       <c r="C170" t="s">
-        <v>1263</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B171" t="s">
-        <v>724</v>
+        <v>3</v>
       </c>
       <c r="C171" t="s">
-        <v>1264</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B172" t="s">
-        <v>724</v>
+        <v>3</v>
       </c>
       <c r="C172" t="s">
-        <v>1265</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B173" t="s">
-        <v>724</v>
+        <v>3</v>
       </c>
       <c r="C173" t="s">
-        <v>1266</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B174" t="s">
-        <v>724</v>
+        <v>3</v>
       </c>
       <c r="C174" t="s">
-        <v>1267</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B175" t="s">
-        <v>724</v>
+        <v>3</v>
       </c>
       <c r="C175" t="s">
-        <v>1268</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B176" t="s">
-        <v>724</v>
+        <v>3</v>
       </c>
       <c r="C176" t="s">
-        <v>1269</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B177" t="s">
-        <v>724</v>
+        <v>3</v>
       </c>
       <c r="C177" t="s">
-        <v>1270</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B178" t="s">
-        <v>724</v>
+        <v>3</v>
       </c>
       <c r="C178" t="s">
-        <v>1271</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179">
+        <v>3</v>
+      </c>
+      <c r="B179" t="s">
+        <v>3</v>
+      </c>
+      <c r="C179" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>3</v>
+      </c>
+      <c r="B180" t="s">
+        <v>3</v>
+      </c>
+      <c r="C180" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>3</v>
+      </c>
+      <c r="B181" t="s">
+        <v>3</v>
+      </c>
+      <c r="C181" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>3</v>
+      </c>
+      <c r="B182" t="s">
+        <v>3</v>
+      </c>
+      <c r="C182" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>3</v>
+      </c>
+      <c r="B183" t="s">
+        <v>3</v>
+      </c>
+      <c r="C183" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>3</v>
+      </c>
+      <c r="B184" t="s">
+        <v>3</v>
+      </c>
+      <c r="C184" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>3</v>
+      </c>
+      <c r="B185" t="s">
+        <v>3</v>
+      </c>
+      <c r="C185" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>3</v>
+      </c>
+      <c r="B186" t="s">
+        <v>3</v>
+      </c>
+      <c r="C186" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>3</v>
+      </c>
+      <c r="B187" t="s">
+        <v>3</v>
+      </c>
+      <c r="C187" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>3</v>
+      </c>
+      <c r="B188" t="s">
+        <v>3</v>
+      </c>
+      <c r="C188" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>3</v>
+      </c>
+      <c r="B189" t="s">
+        <v>3</v>
+      </c>
+      <c r="C189" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>3</v>
+      </c>
+      <c r="B190" t="s">
+        <v>3</v>
+      </c>
+      <c r="C190" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>3</v>
+      </c>
+      <c r="B191" t="s">
+        <v>3</v>
+      </c>
+      <c r="C191" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>3</v>
+      </c>
+      <c r="B192" t="s">
+        <v>3</v>
+      </c>
+      <c r="C192" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>3</v>
+      </c>
+      <c r="B193" t="s">
+        <v>3</v>
+      </c>
+      <c r="C193" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>3</v>
+      </c>
+      <c r="B194" t="s">
+        <v>3</v>
+      </c>
+      <c r="C194" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>3</v>
+      </c>
+      <c r="B195" t="s">
+        <v>3</v>
+      </c>
+      <c r="C195" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A196">
         <v>4</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B196" t="s">
         <v>724</v>
       </c>
-      <c r="C179" t="s">
-        <v>1272</v>
+      <c r="C196" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>4</v>
+      </c>
+      <c r="B197" t="s">
+        <v>724</v>
+      </c>
+      <c r="C197" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>4</v>
+      </c>
+      <c r="B198" t="s">
+        <v>724</v>
+      </c>
+      <c r="C198" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>4</v>
+      </c>
+      <c r="B199" t="s">
+        <v>724</v>
+      </c>
+      <c r="C199" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>4</v>
+      </c>
+      <c r="B200" t="s">
+        <v>724</v>
+      </c>
+      <c r="C200" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <v>4</v>
+      </c>
+      <c r="B201" t="s">
+        <v>724</v>
+      </c>
+      <c r="C201" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>4</v>
+      </c>
+      <c r="B202" t="s">
+        <v>724</v>
+      </c>
+      <c r="C202" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <v>4</v>
+      </c>
+      <c r="B203" t="s">
+        <v>724</v>
+      </c>
+      <c r="C203" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>4</v>
+      </c>
+      <c r="B204" t="s">
+        <v>724</v>
+      </c>
+      <c r="C204" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>4</v>
+      </c>
+      <c r="B205" t="s">
+        <v>724</v>
+      </c>
+      <c r="C205" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>4</v>
+      </c>
+      <c r="B206" t="s">
+        <v>724</v>
+      </c>
+      <c r="C206" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>4</v>
+      </c>
+      <c r="B207" t="s">
+        <v>724</v>
+      </c>
+      <c r="C207" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>4</v>
+      </c>
+      <c r="B208" t="s">
+        <v>724</v>
+      </c>
+      <c r="C208" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>4</v>
+      </c>
+      <c r="B209" t="s">
+        <v>724</v>
+      </c>
+      <c r="C209" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>4</v>
+      </c>
+      <c r="B210" t="s">
+        <v>724</v>
+      </c>
+      <c r="C210" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>4</v>
+      </c>
+      <c r="B211" t="s">
+        <v>724</v>
+      </c>
+      <c r="C211" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>4</v>
+      </c>
+      <c r="B212" t="s">
+        <v>724</v>
+      </c>
+      <c r="C212" t="s">
+        <v>1243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wnrs Couples level 5 added
</commit_message>
<xml_diff>
--- a/data/WNRS.xlsx
+++ b/data/WNRS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KayJan/test-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A801337-F40C-8347-B089-1FAE94CD6B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C9BFFC-3310-C849-AADC-1B5174CD1A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-5320" windowWidth="38400" windowHeight="21100" tabRatio="829" firstSheet="11" activeTab="23" xr2:uid="{35520F66-FEA5-4575-927A-C3FC8E8C1344}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2731" uniqueCount="1308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2765" uniqueCount="1325">
   <si>
     <t>Card</t>
   </si>
@@ -4084,6 +4084,57 @@
   </si>
   <si>
     <t xml:space="preserve">What's your favourite gift I've given you? </t>
+  </si>
+  <si>
+    <t>Will you feel hurt if I start watching a brand new TV series without asking you first if you'd like to join me on the journey?</t>
+  </si>
+  <si>
+    <t>When we order food should I assume we're sharing what's on each other's plate or is your meal off limits to me?</t>
+  </si>
+  <si>
+    <t>Are we generally splitting things down the middle when we pay for stuff or is one of us going to pay more?</t>
+  </si>
+  <si>
+    <t>When it comes to presents, what is your expectations (birthdays, holidays, anniversaries)?</t>
+  </si>
+  <si>
+    <t>Are we to assume that certain days or evenings are always spent together or do I need to lock down plans with you as the week rolls on?</t>
+  </si>
+  <si>
+    <t>Do you have any doubts or fears when you make commitment?</t>
+  </si>
+  <si>
+    <t>Are we going to combine finances or keep things separate? What about a big joint purchase? Do you have any debt?</t>
+  </si>
+  <si>
+    <t>Do you want any kids or want more kids? What about fur babies?</t>
+  </si>
+  <si>
+    <t>Do you want to be in a monogamous relationship forever, a poly relationship forever or leave things open and check in every year?</t>
+  </si>
+  <si>
+    <t>How can we improve our communication? Is there anything I can do that can make it easier for you to bring up difficult topics?</t>
+  </si>
+  <si>
+    <t>Under what circumstances would you start considering divorce?</t>
+  </si>
+  <si>
+    <t>What would you do if you are falling out of love? Would you tell me? Would you tell your therapist or friend first?</t>
+  </si>
+  <si>
+    <t>What do you consider cheating? Is it flirting, make outs, or a close emotional relationship with someone you could be attracted to?</t>
+  </si>
+  <si>
+    <t>What emoji should I include if I'm being funny or sarcastic in a text so you don't get the wrong idea?</t>
+  </si>
+  <si>
+    <t>Should I always take your side when you're complaining about someone you can't stand or should I gently challenge you if I think you're being unfair?</t>
+  </si>
+  <si>
+    <t>How often are we going to see your family? Do you want your parents to move in with us if they eventually need more care?</t>
+  </si>
+  <si>
+    <t>What secrets are okay to keep private? When does omitting information feel deceitful?</t>
   </si>
 </sst>
 </file>
@@ -12321,11 +12372,9 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA8A9E1-0154-BF46-81F5-4F5B0654000C}">
-  <dimension ref="A1:C212"/>
+  <dimension ref="A1:C229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="200" workbookViewId="0">
-      <selection activeCell="C180" sqref="C180"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -14639,6 +14688,193 @@
       </c>
       <c r="C212" t="s">
         <v>1216</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>5</v>
+      </c>
+      <c r="B213" t="s">
+        <v>711</v>
+      </c>
+      <c r="C213" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>5</v>
+      </c>
+      <c r="B214" t="s">
+        <v>711</v>
+      </c>
+      <c r="C214" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>5</v>
+      </c>
+      <c r="B215" t="s">
+        <v>711</v>
+      </c>
+      <c r="C215" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>5</v>
+      </c>
+      <c r="B216" t="s">
+        <v>711</v>
+      </c>
+      <c r="C216" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>5</v>
+      </c>
+      <c r="B217" t="s">
+        <v>711</v>
+      </c>
+      <c r="C217" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>5</v>
+      </c>
+      <c r="B218" t="s">
+        <v>711</v>
+      </c>
+      <c r="C218" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>5</v>
+      </c>
+      <c r="B219" t="s">
+        <v>711</v>
+      </c>
+      <c r="C219" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>5</v>
+      </c>
+      <c r="B220" t="s">
+        <v>711</v>
+      </c>
+      <c r="C220" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>5</v>
+      </c>
+      <c r="B221" t="s">
+        <v>711</v>
+      </c>
+      <c r="C221" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>5</v>
+      </c>
+      <c r="B222" t="s">
+        <v>711</v>
+      </c>
+      <c r="C222" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>5</v>
+      </c>
+      <c r="B223" t="s">
+        <v>711</v>
+      </c>
+      <c r="C223" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>5</v>
+      </c>
+      <c r="B224" t="s">
+        <v>711</v>
+      </c>
+      <c r="C224" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>5</v>
+      </c>
+      <c r="B225" t="s">
+        <v>711</v>
+      </c>
+      <c r="C225" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>5</v>
+      </c>
+      <c r="B226" t="s">
+        <v>711</v>
+      </c>
+      <c r="C226" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <v>5</v>
+      </c>
+      <c r="B227" t="s">
+        <v>711</v>
+      </c>
+      <c r="C227" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <v>5</v>
+      </c>
+      <c r="B228" t="s">
+        <v>711</v>
+      </c>
+      <c r="C228" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>5</v>
+      </c>
+      <c r="B229" t="s">
+        <v>711</v>
+      </c>
+      <c r="C229" t="s">
+        <v>1318</v>
       </c>
     </row>
   </sheetData>
@@ -15133,7 +15369,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -16682,7 +16918,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>

</xml_diff>